<commit_message>
Fixed E. fragilis page and removed extra period after "outreach" from Index page.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/new_spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C929DA-B25E-7F4C-AA1C-7D5E8E4DC48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8506CA71-97B0-534B-A97F-89EE2E0F23DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -6790,8 +6790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7534,14 +7534,14 @@
       <c r="A53" s="18">
         <v>159</v>
       </c>
-      <c r="B53" s="19" t="s">
-        <v>3</v>
+      <c r="B53" s="18">
+        <v>32.884805555555552</v>
       </c>
       <c r="C53" s="18">
-        <v>32.884805555555552</v>
-      </c>
-      <c r="D53" s="18">
         <v>-93.893250000000009</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -8289,7 +8289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F200" sqref="F200"/>
     </sheetView>

</xml_diff>

<commit_message>
Made a correction on the S. lacustris map.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/new_spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8506CA71-97B0-534B-A97F-89EE2E0F23DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F73141-73A9-EE48-A4EA-9E2C56AC7705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="27">
   <si>
     <t>Long</t>
   </si>
@@ -589,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L203"/>
   <sheetViews>
-    <sheetView topLeftCell="A170" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I203" sqref="I203"/>
     </sheetView>
   </sheetViews>
@@ -6790,7 +6790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
@@ -8289,9 +8289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U200"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F200" sqref="F200"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M151" sqref="M151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10871,7 +10871,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" s="12">
         <v>0</v>
@@ -17120,7 +17120,7 @@
       <c r="J151" s="20"/>
       <c r="K151" s="20"/>
       <c r="L151" s="20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M151" s="20"/>
       <c r="N151" s="20">
@@ -20666,10 +20666,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20774,13 +20774,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="B8">
-        <v>30.029249999999998</v>
+        <v>30.539805555555599</v>
       </c>
       <c r="C8">
-        <v>-90.12022222222221</v>
+        <v>-89.874499999999998</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3</v>
@@ -20788,10 +20788,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="B9">
-        <v>30.539805555555599</v>
+        <v>30.539805555555557</v>
       </c>
       <c r="C9">
         <v>-89.874499999999998</v>
@@ -20801,30 +20801,16 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>139</v>
-      </c>
-      <c r="B10">
-        <v>30.539805555555557</v>
-      </c>
-      <c r="C10">
-        <v>-89.874499999999998</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="18">
+      <c r="A10" s="18">
         <v>172</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B10" s="18">
         <v>30.362912222222224</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C10" s="18">
         <v>-89.734103055555551</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D10" s="19" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added sites to the presence/absence map and removed the inaccurate site 33 from the E. fluviatilis map.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/new_spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA67251-6F4B-E542-B4B3-D66A3AC963A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F263D48-26A9-5D42-B3AA-1F2CD8581D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -188,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +198,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,12 +262,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -282,7 +288,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -570,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -578,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L203"/>
+  <dimension ref="A1:L208"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="I208" sqref="I208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4646,7 +4652,7 @@
         <v>15.49</v>
       </c>
       <c r="E135" s="3">
-        <f t="shared" ref="E135:E203" si="18">B135+C135/60+D135/3600</f>
+        <f t="shared" ref="E135:E208" si="18">B135+C135/60+D135/3600</f>
         <v>30.370969444444444</v>
       </c>
       <c r="F135" s="1">
@@ -4659,7 +4665,7 @@
         <v>31.54</v>
       </c>
       <c r="I135">
-        <f t="shared" ref="I135:I203" si="19">-F135-G135/60-H135/3600</f>
+        <f t="shared" ref="I135:I208" si="19">-F135-G135/60-H135/3600</f>
         <v>-91.625427777777773</v>
       </c>
     </row>
@@ -6769,6 +6775,161 @@
       <c r="I203">
         <f t="shared" si="19"/>
         <v>-91.191599722222222</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>199</v>
+      </c>
+      <c r="B204" s="1">
+        <v>30</v>
+      </c>
+      <c r="C204">
+        <v>23</v>
+      </c>
+      <c r="D204">
+        <v>24.096</v>
+      </c>
+      <c r="E204" s="3">
+        <f t="shared" si="18"/>
+        <v>30.390026666666667</v>
+      </c>
+      <c r="F204" s="1">
+        <v>91</v>
+      </c>
+      <c r="G204">
+        <v>2</v>
+      </c>
+      <c r="H204">
+        <v>6.2489999999999997</v>
+      </c>
+      <c r="I204">
+        <f t="shared" si="19"/>
+        <v>-91.035069166666659</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>200</v>
+      </c>
+      <c r="B205" s="1">
+        <v>30</v>
+      </c>
+      <c r="C205">
+        <v>19</v>
+      </c>
+      <c r="D205">
+        <v>16.773</v>
+      </c>
+      <c r="E205" s="3">
+        <f t="shared" si="18"/>
+        <v>30.321325833333333</v>
+      </c>
+      <c r="F205" s="1">
+        <v>91</v>
+      </c>
+      <c r="G205">
+        <v>1</v>
+      </c>
+      <c r="H205">
+        <v>16.928999999999998</v>
+      </c>
+      <c r="I205">
+        <f t="shared" si="19"/>
+        <v>-91.021369166666659</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>201</v>
+      </c>
+      <c r="B206" s="1">
+        <v>30</v>
+      </c>
+      <c r="C206">
+        <v>19</v>
+      </c>
+      <c r="D206">
+        <v>15.884</v>
+      </c>
+      <c r="E206" s="3">
+        <f t="shared" si="18"/>
+        <v>30.321078888888888</v>
+      </c>
+      <c r="F206" s="1">
+        <v>91</v>
+      </c>
+      <c r="G206">
+        <v>1</v>
+      </c>
+      <c r="H206">
+        <v>14.798999999999999</v>
+      </c>
+      <c r="I206">
+        <f t="shared" si="19"/>
+        <v>-91.020777499999994</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>202</v>
+      </c>
+      <c r="B207" s="1">
+        <v>30</v>
+      </c>
+      <c r="C207">
+        <v>24</v>
+      </c>
+      <c r="D207">
+        <v>45.302</v>
+      </c>
+      <c r="E207" s="3">
+        <f t="shared" si="18"/>
+        <v>30.412583888888886</v>
+      </c>
+      <c r="F207" s="1">
+        <v>90</v>
+      </c>
+      <c r="G207">
+        <v>58</v>
+      </c>
+      <c r="H207">
+        <v>29.550999999999998</v>
+      </c>
+      <c r="I207">
+        <f t="shared" si="19"/>
+        <v>-90.974875277777784</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>203</v>
+      </c>
+      <c r="B208" s="1">
+        <v>30</v>
+      </c>
+      <c r="C208">
+        <v>24</v>
+      </c>
+      <c r="D208">
+        <v>43.667999999999999</v>
+      </c>
+      <c r="E208" s="3">
+        <f t="shared" si="18"/>
+        <v>30.412129999999998</v>
+      </c>
+      <c r="F208" s="1">
+        <v>90</v>
+      </c>
+      <c r="G208">
+        <v>58</v>
+      </c>
+      <c r="H208">
+        <v>29.687000000000001</v>
+      </c>
+      <c r="I208">
+        <f t="shared" si="19"/>
+        <v>-90.974913055555561</v>
       </c>
     </row>
   </sheetData>
@@ -6973,10 +7134,10 @@
       <c r="A14">
         <v>52</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14">
         <v>30.362750000000002</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14">
         <v>-90.089333333333329</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -7519,10 +7680,10 @@
       <c r="A53">
         <v>152</v>
       </c>
-      <c r="B53" s="14">
+      <c r="B53">
         <v>31.884277777777779</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53">
         <v>-92.953888888888898</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -7729,10 +7890,10 @@
       <c r="A68">
         <v>186</v>
       </c>
-      <c r="B68" s="14">
+      <c r="B68">
         <v>32.314416666666666</v>
       </c>
-      <c r="C68" s="14">
+      <c r="C68">
         <v>-93.151305555555567</v>
       </c>
       <c r="D68" s="3" t="s">
@@ -7743,10 +7904,10 @@
       <c r="A69">
         <v>188</v>
       </c>
-      <c r="B69" s="14">
+      <c r="B69">
         <v>32.323081666666667</v>
       </c>
-      <c r="C69" s="14">
+      <c r="C69">
         <v>-93.41498555555556</v>
       </c>
       <c r="D69" s="3" t="s">
@@ -7771,10 +7932,10 @@
       <c r="A71">
         <v>196</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B71">
         <v>30.699066944444446</v>
       </c>
-      <c r="C71" s="14">
+      <c r="C71">
         <v>-92.89471166666668</v>
       </c>
       <c r="D71" s="3" t="s">
@@ -7788,10 +7949,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7814,42 +7975,42 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17">
-        <v>33</v>
+      <c r="A2" s="3">
+        <v>52</v>
       </c>
       <c r="B2">
-        <v>30.126750000000001</v>
+        <v>30.362750000000002</v>
       </c>
       <c r="C2">
-        <v>-91.27847222222222</v>
+        <v>-90.089333333333329</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
-        <v>52</v>
-      </c>
-      <c r="B3" s="14">
-        <v>30.362750000000002</v>
-      </c>
-      <c r="C3" s="14">
-        <v>-90.089333333333329</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="A3">
+        <v>83</v>
+      </c>
+      <c r="B3">
+        <v>29.987055555555557</v>
+      </c>
+      <c r="C3">
+        <v>-90.091555555555544</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4">
-        <v>29.987055555555557</v>
+        <v>30.00375</v>
       </c>
       <c r="C4">
-        <v>-90.091555555555544</v>
+        <v>-90.096166666666662</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
@@ -7857,13 +8018,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B5">
-        <v>30.00375</v>
+        <v>29.983249999999998</v>
       </c>
       <c r="C5">
-        <v>-90.096166666666662</v>
+        <v>-90.090305555555545</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
@@ -7871,13 +8032,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B6">
-        <v>29.983249999999998</v>
+        <v>30.02547222222222</v>
       </c>
       <c r="C6">
-        <v>-90.090305555555545</v>
+        <v>-90.115638888888881</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
@@ -7885,13 +8046,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>92</v>
+        <v>141</v>
       </c>
       <c r="B7">
-        <v>30.02547222222222</v>
-      </c>
-      <c r="C7">
-        <v>-90.115638888888881</v>
+        <v>30.0215</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-90.15313888888889</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>3</v>
@@ -7899,13 +8060,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B8">
-        <v>30.0215</v>
-      </c>
-      <c r="C8" s="3">
-        <v>-90.15313888888889</v>
+        <v>30.026527777777776</v>
+      </c>
+      <c r="C8">
+        <v>-90.08197222222222</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>3</v>
@@ -7913,29 +8074,15 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B9">
-        <v>30.026527777777776</v>
+        <v>30.06527777777778</v>
       </c>
       <c r="C9">
-        <v>-90.08197222222222</v>
+        <v>-89.806527777777774</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>144</v>
-      </c>
-      <c r="B10">
-        <v>30.06527777777778</v>
-      </c>
-      <c r="C10">
-        <v>-89.806527777777774</v>
-      </c>
-      <c r="D10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7949,7 +8096,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8112,10 +8259,10 @@
       <c r="A12">
         <v>152</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12">
         <v>31.884277777777779</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12">
         <v>-92.953888888888898</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -8412,7 +8559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8480,11 +8627,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U200"/>
+  <dimension ref="A1:U205"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C183" sqref="C183:D183"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10408,10 +10555,10 @@
         <v>1</v>
       </c>
       <c r="N34" s="10">
+        <v>0</v>
+      </c>
+      <c r="O34" s="10">
         <v>2</v>
-      </c>
-      <c r="O34" s="10">
-        <v>0</v>
       </c>
       <c r="P34" s="10">
         <v>0</v>
@@ -12708,49 +12855,49 @@
       <c r="D77">
         <v>-91.827305555555554</v>
       </c>
-      <c r="F77" s="15">
-        <v>0</v>
-      </c>
-      <c r="G77" s="15">
-        <v>0</v>
-      </c>
-      <c r="H77" s="15">
-        <v>0</v>
-      </c>
-      <c r="I77" s="15">
-        <v>0</v>
-      </c>
-      <c r="J77" s="15">
-        <v>0</v>
-      </c>
-      <c r="K77" s="15">
-        <v>0</v>
-      </c>
-      <c r="L77" s="15">
-        <v>0</v>
-      </c>
-      <c r="M77" s="15">
-        <v>0</v>
-      </c>
-      <c r="N77" s="15">
-        <v>0</v>
-      </c>
-      <c r="O77" s="15">
-        <v>0</v>
-      </c>
-      <c r="P77" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q77" s="15">
-        <v>0</v>
-      </c>
-      <c r="R77" s="15">
-        <v>0</v>
-      </c>
-      <c r="S77" s="15">
-        <v>0</v>
-      </c>
-      <c r="T77" s="15">
+      <c r="F77" s="14">
+        <v>0</v>
+      </c>
+      <c r="G77" s="14">
+        <v>0</v>
+      </c>
+      <c r="H77" s="14">
+        <v>0</v>
+      </c>
+      <c r="I77" s="14">
+        <v>0</v>
+      </c>
+      <c r="J77" s="14">
+        <v>0</v>
+      </c>
+      <c r="K77" s="14">
+        <v>0</v>
+      </c>
+      <c r="L77" s="14">
+        <v>0</v>
+      </c>
+      <c r="M77" s="14">
+        <v>0</v>
+      </c>
+      <c r="N77" s="14">
+        <v>0</v>
+      </c>
+      <c r="O77" s="14">
+        <v>0</v>
+      </c>
+      <c r="P77" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="14">
+        <v>0</v>
+      </c>
+      <c r="R77" s="14">
+        <v>0</v>
+      </c>
+      <c r="S77" s="14">
+        <v>0</v>
+      </c>
+      <c r="T77" s="14">
         <v>0</v>
       </c>
     </row>
@@ -16595,7 +16742,7 @@
       </c>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A149" s="14">
+      <c r="A149">
         <v>147</v>
       </c>
       <c r="B149" s="3" t="s">
@@ -16654,7 +16801,7 @@
       </c>
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A150" s="14">
+      <c r="A150">
         <v>148</v>
       </c>
       <c r="B150" s="3" t="s">
@@ -16713,7 +16860,7 @@
       </c>
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A151" s="14">
+      <c r="A151">
         <v>149</v>
       </c>
       <c r="B151" s="3" t="s">
@@ -16803,7 +16950,7 @@
       <c r="T152" s="13"/>
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A153" s="14">
+      <c r="A153">
         <v>151</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -17074,7 +17221,7 @@
       </c>
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A158" s="14">
+      <c r="A158">
         <v>156</v>
       </c>
       <c r="B158" s="3" t="s">
@@ -17133,7 +17280,7 @@
       </c>
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A159" s="14">
+      <c r="A159">
         <v>157</v>
       </c>
       <c r="B159" s="3" t="s">
@@ -17192,7 +17339,7 @@
       </c>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A160" s="14">
+      <c r="A160">
         <v>158</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -17564,7 +17711,7 @@
       <c r="T167" s="13"/>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A168" s="14">
+      <c r="A168">
         <v>166</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -18210,7 +18357,7 @@
       <c r="T181" s="13"/>
     </row>
     <row r="182" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A182" s="14">
+      <c r="A182">
         <v>180</v>
       </c>
       <c r="B182" s="3" t="s">
@@ -18269,7 +18416,7 @@
       </c>
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A183" s="14">
+      <c r="A183">
         <v>181</v>
       </c>
       <c r="B183" s="3" t="s">
@@ -18357,7 +18504,7 @@
       <c r="T184" s="13"/>
     </row>
     <row r="185" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A185" s="14">
+      <c r="A185">
         <v>183</v>
       </c>
       <c r="B185" s="3" t="s">
@@ -18416,7 +18563,7 @@
       </c>
     </row>
     <row r="186" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A186" s="14">
+      <c r="A186">
         <v>184</v>
       </c>
       <c r="B186" s="3" t="s">
@@ -18636,7 +18783,7 @@
       <c r="T191" s="13"/>
     </row>
     <row r="192" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A192" s="14">
+      <c r="A192">
         <v>190</v>
       </c>
       <c r="B192" s="3" t="s">
@@ -18695,7 +18842,7 @@
       </c>
     </row>
     <row r="193" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A193" s="14">
+      <c r="A193">
         <v>191</v>
       </c>
       <c r="B193" s="3" t="s">
@@ -18754,7 +18901,7 @@
       </c>
     </row>
     <row r="194" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A194" s="14">
+      <c r="A194">
         <v>192</v>
       </c>
       <c r="B194" s="3" t="s">
@@ -18813,7 +18960,7 @@
       </c>
     </row>
     <row r="195" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A195" s="14">
+      <c r="A195">
         <v>193</v>
       </c>
       <c r="B195" s="3" t="s">
@@ -18872,7 +19019,7 @@
       </c>
     </row>
     <row r="196" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A196" s="14">
+      <c r="A196">
         <v>194</v>
       </c>
       <c r="B196" s="3" t="s">
@@ -18991,7 +19138,7 @@
       <c r="T198" s="13"/>
     </row>
     <row r="199" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A199" s="14">
+      <c r="A199">
         <v>197</v>
       </c>
       <c r="B199" s="3" t="s">
@@ -19050,7 +19197,7 @@
       </c>
     </row>
     <row r="200" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A200" s="14">
+      <c r="A200">
         <v>198</v>
       </c>
       <c r="B200" s="3" t="s">
@@ -19105,6 +19252,166 @@
         <v>0</v>
       </c>
       <c r="T200" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="16">
+        <v>199</v>
+      </c>
+      <c r="B201" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="16">
+        <v>30.390026666666667</v>
+      </c>
+      <c r="D201" s="16">
+        <v>-91.035069166666659</v>
+      </c>
+    </row>
+    <row r="202" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="16">
+        <v>200</v>
+      </c>
+      <c r="B202" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C202" s="16">
+        <v>30.321325833333333</v>
+      </c>
+      <c r="D202" s="16">
+        <v>-91.021369166666659</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="16">
+        <v>201</v>
+      </c>
+      <c r="B203" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C203" s="16">
+        <v>30.321078888888888</v>
+      </c>
+      <c r="D203" s="16">
+        <v>-91.020777499999994</v>
+      </c>
+      <c r="F203" s="16">
+        <v>0</v>
+      </c>
+      <c r="G203" s="16">
+        <v>0</v>
+      </c>
+      <c r="H203" s="16">
+        <v>0</v>
+      </c>
+      <c r="I203" s="16">
+        <v>0</v>
+      </c>
+      <c r="J203" s="16">
+        <v>0</v>
+      </c>
+      <c r="K203" s="16">
+        <v>0</v>
+      </c>
+      <c r="L203" s="16">
+        <v>0</v>
+      </c>
+      <c r="M203" s="16">
+        <v>0</v>
+      </c>
+      <c r="N203" s="16">
+        <v>0</v>
+      </c>
+      <c r="O203" s="16">
+        <v>0</v>
+      </c>
+      <c r="P203" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q203" s="16">
+        <v>0</v>
+      </c>
+      <c r="R203" s="16">
+        <v>0</v>
+      </c>
+      <c r="S203" s="16">
+        <v>0</v>
+      </c>
+      <c r="T203" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="16">
+        <v>202</v>
+      </c>
+      <c r="B204" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204" s="16">
+        <v>30.412583888888886</v>
+      </c>
+      <c r="D204" s="16">
+        <v>-90.974875277777784</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="16">
+        <v>203</v>
+      </c>
+      <c r="B205" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205" s="16">
+        <v>30.412129999999998</v>
+      </c>
+      <c r="D205" s="16">
+        <v>-90.974913055555561</v>
+      </c>
+      <c r="F205" s="16">
+        <v>0</v>
+      </c>
+      <c r="G205" s="16">
+        <v>0</v>
+      </c>
+      <c r="H205" s="16">
+        <v>0</v>
+      </c>
+      <c r="I205" s="16">
+        <v>0</v>
+      </c>
+      <c r="J205" s="16">
+        <v>0</v>
+      </c>
+      <c r="K205" s="16">
+        <v>0</v>
+      </c>
+      <c r="L205" s="16">
+        <v>0</v>
+      </c>
+      <c r="M205" s="16">
+        <v>0</v>
+      </c>
+      <c r="N205" s="16">
+        <v>0</v>
+      </c>
+      <c r="O205" s="16">
+        <v>0</v>
+      </c>
+      <c r="P205" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q205" s="16">
+        <v>0</v>
+      </c>
+      <c r="R205" s="16">
+        <v>0</v>
+      </c>
+      <c r="S205" s="16">
+        <v>0</v>
+      </c>
+      <c r="T205" s="16">
         <v>0</v>
       </c>
     </row>
@@ -19190,10 +19497,10 @@
       <c r="A5" s="3">
         <v>59</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5">
         <v>30.375444444444444</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5">
         <v>-89.738888888888894</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -19498,10 +19805,10 @@
       <c r="A27">
         <v>161</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27">
         <v>32.583527777777782</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27">
         <v>-92.070805555555552</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -19769,10 +20076,10 @@
       <c r="A12" s="3">
         <v>54</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12">
         <v>30.480249999999998</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12">
         <v>-90.03991666666667</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -19783,10 +20090,10 @@
       <c r="A13" s="3">
         <v>59</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13">
         <v>30.375444444444444</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13">
         <v>-89.738888888888894</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -19867,10 +20174,10 @@
       <c r="A19" s="3">
         <v>106</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19">
         <v>31.483055555555556</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19">
         <v>-91.8611111111111</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -20381,10 +20688,10 @@
       <c r="A34" s="3">
         <v>106</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34">
         <v>31.483055555555556</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34">
         <v>-91.8611111111111</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -20395,10 +20702,10 @@
       <c r="A35" s="3">
         <v>108</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35">
         <v>31.333888888888886</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35">
         <v>-91.936388888888899</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -20619,10 +20926,10 @@
       <c r="A51">
         <v>151</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B51">
         <v>31.997694444444445</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51">
         <v>-92.896416666666667</v>
       </c>
       <c r="D51" s="3" t="s">
@@ -20633,10 +20940,10 @@
       <c r="A52">
         <v>152</v>
       </c>
-      <c r="B52" s="14">
+      <c r="B52">
         <v>31.884277777777779</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52">
         <v>-92.953888888888898</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -20787,10 +21094,10 @@
       <c r="A63" s="3">
         <v>185</v>
       </c>
-      <c r="B63" s="14">
+      <c r="B63">
         <v>32.171768055555553</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63">
         <v>-92.992765833333337</v>
       </c>
       <c r="D63" s="3" t="s">
@@ -20801,10 +21108,10 @@
       <c r="A64" s="3">
         <v>186</v>
       </c>
-      <c r="B64" s="14">
+      <c r="B64">
         <v>32.314416666666666</v>
       </c>
-      <c r="C64" s="14">
+      <c r="C64">
         <v>-93.151305555555567</v>
       </c>
       <c r="D64" s="3" t="s">
@@ -20815,10 +21122,10 @@
       <c r="A65" s="3">
         <v>187</v>
       </c>
-      <c r="B65" s="14">
+      <c r="B65">
         <v>32.597631666666672</v>
       </c>
-      <c r="C65" s="14">
+      <c r="C65">
         <v>-93.333229722222214</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -20829,10 +21136,10 @@
       <c r="A66" s="3">
         <v>188</v>
       </c>
-      <c r="B66" s="14">
+      <c r="B66">
         <v>32.323081666666667</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C66">
         <v>-93.41498555555556</v>
       </c>
       <c r="D66" s="3" t="s">
@@ -21117,10 +21424,10 @@
       <c r="A13" s="3">
         <v>188</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13">
         <v>32.323081666666667</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13">
         <v>-93.41498555555556</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -21294,10 +21601,10 @@
       <c r="A8">
         <v>54</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8">
         <v>30.480249999999998</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8">
         <v>-90.03991666666667</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -21322,10 +21629,10 @@
       <c r="A10">
         <v>123</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10">
         <v>32.782611099999997</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10">
         <v>-92.490806000000006</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -21392,10 +21699,10 @@
       <c r="A15">
         <v>186</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>32.314416666666666</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <v>-93.151305555555567</v>
       </c>
       <c r="D15" s="3" t="s">

</xml_diff>

<commit_message>
Updates made to the "Meet the Lab" page: Changed the picture at the top, added Jada and moved Jaylon to Previous Undergraduate Researchers. Also, added more sites to the maps.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/new_spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F263D48-26A9-5D42-B3AA-1F2CD8581D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130D38EF-355C-0B42-9CA4-28D7A8AE7D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -229,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
@@ -268,6 +268,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -584,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L208"/>
+  <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="I208" sqref="I208"/>
+    <sheetView topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="E217" sqref="E217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4652,7 +4657,7 @@
         <v>15.49</v>
       </c>
       <c r="E135" s="3">
-        <f t="shared" ref="E135:E208" si="18">B135+C135/60+D135/3600</f>
+        <f t="shared" ref="E135:E217" si="18">B135+C135/60+D135/3600</f>
         <v>30.370969444444444</v>
       </c>
       <c r="F135" s="1">
@@ -4665,7 +4670,7 @@
         <v>31.54</v>
       </c>
       <c r="I135">
-        <f t="shared" ref="I135:I208" si="19">-F135-G135/60-H135/3600</f>
+        <f t="shared" ref="I135:I217" si="19">-F135-G135/60-H135/3600</f>
         <v>-91.625427777777773</v>
       </c>
     </row>
@@ -6930,6 +6935,285 @@
       <c r="I208">
         <f t="shared" si="19"/>
         <v>-90.974913055555561</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>204</v>
+      </c>
+      <c r="B209" s="1">
+        <v>30</v>
+      </c>
+      <c r="C209">
+        <v>2</v>
+      </c>
+      <c r="D209">
+        <v>35.552399999999999</v>
+      </c>
+      <c r="E209" s="3">
+        <f t="shared" si="18"/>
+        <v>30.043209000000001</v>
+      </c>
+      <c r="F209" s="1">
+        <v>90</v>
+      </c>
+      <c r="G209">
+        <v>14</v>
+      </c>
+      <c r="H209">
+        <v>16.194600000000001</v>
+      </c>
+      <c r="I209">
+        <f t="shared" si="19"/>
+        <v>-90.237831833333331</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>205</v>
+      </c>
+      <c r="B210" s="1">
+        <v>30</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+      <c r="D210">
+        <v>13.360799999999999</v>
+      </c>
+      <c r="E210" s="3">
+        <f t="shared" si="18"/>
+        <v>30.020377999999997</v>
+      </c>
+      <c r="F210" s="1">
+        <v>90</v>
+      </c>
+      <c r="G210">
+        <v>8</v>
+      </c>
+      <c r="H210">
+        <v>33.194400000000002</v>
+      </c>
+      <c r="I210">
+        <f t="shared" si="19"/>
+        <v>-90.142554000000004</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>206</v>
+      </c>
+      <c r="B211" s="1">
+        <v>30</v>
+      </c>
+      <c r="C211">
+        <v>6</v>
+      </c>
+      <c r="D211">
+        <v>5.4252000000000002</v>
+      </c>
+      <c r="E211" s="3">
+        <f t="shared" si="18"/>
+        <v>30.101507000000002</v>
+      </c>
+      <c r="F211" s="1">
+        <v>90</v>
+      </c>
+      <c r="G211">
+        <v>44</v>
+      </c>
+      <c r="H211">
+        <v>5.5895999999999999</v>
+      </c>
+      <c r="I211">
+        <f t="shared" si="19"/>
+        <v>-90.734886000000003</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>107</v>
+      </c>
+      <c r="B212" s="1">
+        <v>30</v>
+      </c>
+      <c r="C212">
+        <v>6</v>
+      </c>
+      <c r="D212">
+        <v>3.7547999999999999</v>
+      </c>
+      <c r="E212" s="3">
+        <f t="shared" si="18"/>
+        <v>30.101043000000001</v>
+      </c>
+      <c r="F212" s="1">
+        <v>90</v>
+      </c>
+      <c r="G212">
+        <v>44</v>
+      </c>
+      <c r="H212">
+        <v>12.652200000000001</v>
+      </c>
+      <c r="I212">
+        <f t="shared" si="19"/>
+        <v>-90.736847833333329</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>208</v>
+      </c>
+      <c r="B213" s="1">
+        <v>29</v>
+      </c>
+      <c r="C213">
+        <v>35</v>
+      </c>
+      <c r="D213">
+        <v>56.106000000000002</v>
+      </c>
+      <c r="E213" s="3">
+        <f t="shared" si="18"/>
+        <v>29.598918333333334</v>
+      </c>
+      <c r="F213" s="1">
+        <v>90</v>
+      </c>
+      <c r="G213">
+        <v>42</v>
+      </c>
+      <c r="H213">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="I213">
+        <f t="shared" si="19"/>
+        <v>-90.710750000000004</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>209</v>
+      </c>
+      <c r="B214" s="1">
+        <v>29</v>
+      </c>
+      <c r="C214">
+        <v>34</v>
+      </c>
+      <c r="D214">
+        <v>42.082000000000001</v>
+      </c>
+      <c r="E214" s="3">
+        <f t="shared" si="18"/>
+        <v>29.578356111111113</v>
+      </c>
+      <c r="F214" s="1">
+        <v>90</v>
+      </c>
+      <c r="G214">
+        <v>43</v>
+      </c>
+      <c r="H214">
+        <v>16.978999999999999</v>
+      </c>
+      <c r="I214">
+        <f t="shared" si="19"/>
+        <v>-90.721383055555563</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>210</v>
+      </c>
+      <c r="B215" s="1">
+        <v>29</v>
+      </c>
+      <c r="C215">
+        <v>35</v>
+      </c>
+      <c r="D215">
+        <v>9.9559999999999995</v>
+      </c>
+      <c r="E215" s="3">
+        <f t="shared" si="18"/>
+        <v>29.586098888888888</v>
+      </c>
+      <c r="F215" s="1">
+        <v>90</v>
+      </c>
+      <c r="G215">
+        <v>45</v>
+      </c>
+      <c r="H215">
+        <v>10.564</v>
+      </c>
+      <c r="I215">
+        <f t="shared" si="19"/>
+        <v>-90.752934444444449</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>211</v>
+      </c>
+      <c r="B216" s="1">
+        <v>29</v>
+      </c>
+      <c r="C216">
+        <v>33</v>
+      </c>
+      <c r="D216">
+        <v>39.676000000000002</v>
+      </c>
+      <c r="E216" s="3">
+        <f t="shared" si="18"/>
+        <v>29.561021111111113</v>
+      </c>
+      <c r="F216" s="1">
+        <v>90</v>
+      </c>
+      <c r="G216">
+        <v>47</v>
+      </c>
+      <c r="H216">
+        <v>29.687000000000001</v>
+      </c>
+      <c r="I216">
+        <f t="shared" si="19"/>
+        <v>-90.791579722222224</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>212</v>
+      </c>
+      <c r="B217" s="1">
+        <v>29</v>
+      </c>
+      <c r="C217">
+        <v>32</v>
+      </c>
+      <c r="D217">
+        <v>53.112000000000002</v>
+      </c>
+      <c r="E217" s="3">
+        <f t="shared" si="18"/>
+        <v>29.54808666666667</v>
+      </c>
+      <c r="F217" s="1">
+        <v>90</v>
+      </c>
+      <c r="G217">
+        <v>47</v>
+      </c>
+      <c r="H217">
+        <v>28.664000000000001</v>
+      </c>
+      <c r="I217">
+        <f t="shared" si="19"/>
+        <v>-90.79129555555555</v>
       </c>
     </row>
   </sheetData>
@@ -6940,10 +7224,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:C71"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7939,6 +8223,34 @@
         <v>-92.89471166666668</v>
       </c>
       <c r="D71" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>200</v>
+      </c>
+      <c r="B72">
+        <v>30.321325833333333</v>
+      </c>
+      <c r="C72">
+        <v>-91.021369166666659</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>202</v>
+      </c>
+      <c r="B73">
+        <v>30.412583888888886</v>
+      </c>
+      <c r="C73">
+        <v>-90.974875277777784</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7951,7 +8263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -8627,11 +8939,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U205"/>
+  <dimension ref="A1:U214"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:D34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G217" sqref="G217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19255,163 +19567,472 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="16">
+    <row r="201" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="9">
         <v>199</v>
       </c>
-      <c r="B201" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C201" s="16">
+      <c r="B201" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="9">
         <v>30.390026666666667</v>
       </c>
-      <c r="D201" s="16">
+      <c r="D201" s="9">
         <v>-91.035069166666659</v>
       </c>
     </row>
-    <row r="202" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="16">
+    <row r="202" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="9">
         <v>200</v>
       </c>
-      <c r="B202" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C202" s="16">
+      <c r="B202" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C202" s="9">
         <v>30.321325833333333</v>
       </c>
-      <c r="D202" s="16">
+      <c r="D202" s="9">
         <v>-91.021369166666659</v>
       </c>
-    </row>
-    <row r="203" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="16">
+      <c r="M202" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A203">
         <v>201</v>
       </c>
-      <c r="B203" s="17" t="s">
+      <c r="B203" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C203" s="16">
+      <c r="C203">
         <v>30.321078888888888</v>
       </c>
-      <c r="D203" s="16">
+      <c r="D203">
         <v>-91.020777499999994</v>
       </c>
-      <c r="F203" s="16">
-        <v>0</v>
-      </c>
-      <c r="G203" s="16">
-        <v>0</v>
-      </c>
-      <c r="H203" s="16">
-        <v>0</v>
-      </c>
-      <c r="I203" s="16">
-        <v>0</v>
-      </c>
-      <c r="J203" s="16">
-        <v>0</v>
-      </c>
-      <c r="K203" s="16">
-        <v>0</v>
-      </c>
-      <c r="L203" s="16">
-        <v>0</v>
-      </c>
-      <c r="M203" s="16">
-        <v>0</v>
-      </c>
-      <c r="N203" s="16">
-        <v>0</v>
-      </c>
-      <c r="O203" s="16">
-        <v>0</v>
-      </c>
-      <c r="P203" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q203" s="16">
-        <v>0</v>
-      </c>
-      <c r="R203" s="16">
-        <v>0</v>
-      </c>
-      <c r="S203" s="16">
-        <v>0</v>
-      </c>
-      <c r="T203" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="16">
+      <c r="F203">
+        <v>0</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>0</v>
+      </c>
+      <c r="I203">
+        <v>0</v>
+      </c>
+      <c r="J203">
+        <v>0</v>
+      </c>
+      <c r="K203">
+        <v>0</v>
+      </c>
+      <c r="L203">
+        <v>0</v>
+      </c>
+      <c r="M203">
+        <v>0</v>
+      </c>
+      <c r="N203">
+        <v>0</v>
+      </c>
+      <c r="O203">
+        <v>0</v>
+      </c>
+      <c r="P203">
+        <v>0</v>
+      </c>
+      <c r="Q203">
+        <v>0</v>
+      </c>
+      <c r="R203">
+        <v>0</v>
+      </c>
+      <c r="S203">
+        <v>0</v>
+      </c>
+      <c r="T203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A204">
         <v>202</v>
       </c>
-      <c r="B204" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C204" s="16">
+      <c r="B204" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204">
         <v>30.412583888888886</v>
       </c>
-      <c r="D204" s="16">
+      <c r="D204">
         <v>-90.974875277777784</v>
       </c>
-    </row>
-    <row r="205" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="16">
+      <c r="F204">
+        <v>0</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>1</v>
+      </c>
+      <c r="I204">
+        <v>0</v>
+      </c>
+      <c r="J204">
+        <v>0</v>
+      </c>
+      <c r="K204">
+        <v>0</v>
+      </c>
+      <c r="L204">
+        <v>0</v>
+      </c>
+      <c r="M204">
+        <v>1</v>
+      </c>
+      <c r="N204">
+        <v>0</v>
+      </c>
+      <c r="O204">
+        <v>0</v>
+      </c>
+      <c r="P204">
+        <v>0</v>
+      </c>
+      <c r="Q204">
+        <v>0</v>
+      </c>
+      <c r="R204">
+        <v>0</v>
+      </c>
+      <c r="S204">
+        <v>0</v>
+      </c>
+      <c r="T204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A205">
         <v>203</v>
       </c>
-      <c r="B205" s="17" t="s">
+      <c r="B205" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C205" s="16">
+      <c r="C205">
         <v>30.412129999999998</v>
       </c>
-      <c r="D205" s="16">
+      <c r="D205">
         <v>-90.974913055555561</v>
       </c>
-      <c r="F205" s="16">
-        <v>0</v>
-      </c>
-      <c r="G205" s="16">
-        <v>0</v>
-      </c>
-      <c r="H205" s="16">
-        <v>0</v>
-      </c>
-      <c r="I205" s="16">
-        <v>0</v>
-      </c>
-      <c r="J205" s="16">
-        <v>0</v>
-      </c>
-      <c r="K205" s="16">
-        <v>0</v>
-      </c>
-      <c r="L205" s="16">
-        <v>0</v>
-      </c>
-      <c r="M205" s="16">
-        <v>0</v>
-      </c>
-      <c r="N205" s="16">
-        <v>0</v>
-      </c>
-      <c r="O205" s="16">
-        <v>0</v>
-      </c>
-      <c r="P205" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q205" s="16">
-        <v>0</v>
-      </c>
-      <c r="R205" s="16">
-        <v>0</v>
-      </c>
-      <c r="S205" s="16">
-        <v>0</v>
-      </c>
-      <c r="T205" s="16">
+      <c r="F205">
+        <v>0</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205">
+        <v>0</v>
+      </c>
+      <c r="I205">
+        <v>0</v>
+      </c>
+      <c r="J205">
+        <v>0</v>
+      </c>
+      <c r="K205">
+        <v>0</v>
+      </c>
+      <c r="L205">
+        <v>0</v>
+      </c>
+      <c r="M205">
+        <v>0</v>
+      </c>
+      <c r="N205">
+        <v>0</v>
+      </c>
+      <c r="O205">
+        <v>0</v>
+      </c>
+      <c r="P205">
+        <v>0</v>
+      </c>
+      <c r="Q205">
+        <v>0</v>
+      </c>
+      <c r="R205">
+        <v>0</v>
+      </c>
+      <c r="S205">
+        <v>0</v>
+      </c>
+      <c r="T205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="9">
+        <v>204</v>
+      </c>
+      <c r="B206" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C206" s="9">
+        <v>30.043209000000001</v>
+      </c>
+      <c r="D206" s="9">
+        <v>-90.237831999999997</v>
+      </c>
+    </row>
+    <row r="207" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="9">
+        <v>205</v>
+      </c>
+      <c r="B207" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="9">
+        <v>30.020377700000001</v>
+      </c>
+      <c r="D207" s="9">
+        <v>-90.142554000000004</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="9">
+        <v>206</v>
+      </c>
+      <c r="B208" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C208" s="9">
+        <v>30.101507300000002</v>
+      </c>
+      <c r="D208" s="9">
+        <v>-90.734886500000002</v>
+      </c>
+    </row>
+    <row r="209" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="19">
+        <v>207</v>
+      </c>
+      <c r="B209" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C209" s="19">
+        <v>30.101043000000001</v>
+      </c>
+      <c r="D209" s="19">
+        <v>-90.736847699999998</v>
+      </c>
+      <c r="F209" s="19">
+        <v>0</v>
+      </c>
+      <c r="G209" s="19">
+        <v>0</v>
+      </c>
+      <c r="H209" s="19">
+        <v>0</v>
+      </c>
+      <c r="I209" s="19">
+        <v>0</v>
+      </c>
+      <c r="J209" s="19">
+        <v>0</v>
+      </c>
+      <c r="K209" s="19">
+        <v>0</v>
+      </c>
+      <c r="L209" s="19">
+        <v>0</v>
+      </c>
+      <c r="M209" s="19">
+        <v>0</v>
+      </c>
+      <c r="N209" s="19">
+        <v>0</v>
+      </c>
+      <c r="O209" s="19">
+        <v>0</v>
+      </c>
+      <c r="P209" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q209" s="19">
+        <v>0</v>
+      </c>
+      <c r="R209" s="19">
+        <v>0</v>
+      </c>
+      <c r="S209" s="19">
+        <v>0</v>
+      </c>
+      <c r="T209" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="16">
+        <v>208</v>
+      </c>
+      <c r="B210" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210" s="16">
+        <v>29.598918333333334</v>
+      </c>
+      <c r="D210" s="16">
+        <v>-90.710750000000004</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="16">
+        <v>209</v>
+      </c>
+      <c r="B211" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211" s="16">
+        <v>29.578356111111113</v>
+      </c>
+      <c r="D211" s="16">
+        <v>-90.721383055555563</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="16">
+        <v>210</v>
+      </c>
+      <c r="B212" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C212" s="16">
+        <v>29.586098888888888</v>
+      </c>
+      <c r="D212" s="16">
+        <v>-90.752934444444449</v>
+      </c>
+      <c r="F212" s="16">
+        <v>0</v>
+      </c>
+      <c r="G212" s="16">
+        <v>0</v>
+      </c>
+      <c r="H212" s="16">
+        <v>0</v>
+      </c>
+      <c r="I212" s="16">
+        <v>0</v>
+      </c>
+      <c r="J212" s="16">
+        <v>0</v>
+      </c>
+      <c r="K212" s="16">
+        <v>0</v>
+      </c>
+      <c r="L212" s="16">
+        <v>0</v>
+      </c>
+      <c r="M212" s="16">
+        <v>0</v>
+      </c>
+      <c r="N212" s="16">
+        <v>0</v>
+      </c>
+      <c r="O212" s="16">
+        <v>0</v>
+      </c>
+      <c r="P212" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q212" s="16">
+        <v>0</v>
+      </c>
+      <c r="R212" s="16">
+        <v>0</v>
+      </c>
+      <c r="S212" s="16">
+        <v>0</v>
+      </c>
+      <c r="T212" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="16">
+        <v>211</v>
+      </c>
+      <c r="B213" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213" s="16">
+        <v>29.561021111111113</v>
+      </c>
+      <c r="D213" s="16">
+        <v>-90.791579722222224</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="16">
+        <v>212</v>
+      </c>
+      <c r="B214" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C214" s="16">
+        <v>29.54808666666667</v>
+      </c>
+      <c r="D214" s="16">
+        <v>-90.79129555555555</v>
+      </c>
+      <c r="F214" s="16">
+        <v>0</v>
+      </c>
+      <c r="G214" s="16">
+        <v>0</v>
+      </c>
+      <c r="H214" s="16">
+        <v>0</v>
+      </c>
+      <c r="I214" s="16">
+        <v>0</v>
+      </c>
+      <c r="J214" s="16">
+        <v>0</v>
+      </c>
+      <c r="K214" s="16">
+        <v>0</v>
+      </c>
+      <c r="L214" s="16">
+        <v>0</v>
+      </c>
+      <c r="M214" s="16">
+        <v>0</v>
+      </c>
+      <c r="N214" s="16">
+        <v>0</v>
+      </c>
+      <c r="O214" s="16">
+        <v>0</v>
+      </c>
+      <c r="P214" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q214" s="16">
+        <v>0</v>
+      </c>
+      <c r="R214" s="16">
+        <v>0</v>
+      </c>
+      <c r="S214" s="16">
+        <v>0</v>
+      </c>
+      <c r="T214" s="16">
         <v>0</v>
       </c>
     </row>
@@ -20205,10 +20826,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:C66"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21143,6 +21764,20 @@
         <v>-93.41498555555556</v>
       </c>
       <c r="D66" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>202</v>
+      </c>
+      <c r="B67" s="18">
+        <v>30.412583999999999</v>
+      </c>
+      <c r="C67" s="18">
+        <v>-90.974874999999997</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Abhi's bio on the "Meet the Lab" page. Also, added more sites to any maps that needed to be updated.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/new_spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130D38EF-355C-0B42-9CA4-28D7A8AE7D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36942384-226F-DB43-8AB3-A6DD66082AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -188,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,12 +198,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -229,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
@@ -266,15 +260,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7224,10 +7215,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8254,6 +8245,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="17">
+        <v>208</v>
+      </c>
+      <c r="B74" s="17">
+        <v>29.598918333333334</v>
+      </c>
+      <c r="C74" s="17">
+        <v>-90.710750000000004</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="17">
+        <v>209</v>
+      </c>
+      <c r="B75" s="17">
+        <v>29.578356111111113</v>
+      </c>
+      <c r="C75" s="17">
+        <v>-90.721383055555563</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="17">
+        <v>211</v>
+      </c>
+      <c r="B76" s="17">
+        <v>29.561021111111113</v>
+      </c>
+      <c r="C76" s="17">
+        <v>-90.791579722222224</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8261,10 +8294,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8395,6 +8428,20 @@
         <v>-89.806527777777774</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
+        <v>205</v>
+      </c>
+      <c r="B10" s="17">
+        <v>30.020377700000001</v>
+      </c>
+      <c r="C10" s="17">
+        <v>-90.142554000000004</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8741,10 +8788,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8816,6 +8863,34 @@
         <v>-90.08197222222222</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="17">
+        <v>204</v>
+      </c>
+      <c r="B6" s="17">
+        <v>30.043209000000001</v>
+      </c>
+      <c r="C6" s="17">
+        <v>-90.237831999999997</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="17">
+        <v>205</v>
+      </c>
+      <c r="B7" s="17">
+        <v>30.020377700000001</v>
+      </c>
+      <c r="C7" s="17">
+        <v>-90.142554000000004</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8942,8 +9017,8 @@
   <dimension ref="A1:U214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G217" sqref="G217"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A213" sqref="A213:D213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15208,7 +15283,7 @@
       <c r="F114" s="13"/>
       <c r="G114" s="13"/>
       <c r="H114" s="13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I114" s="13"/>
       <c r="J114" s="13">
@@ -17246,7 +17321,7 @@
       <c r="F152" s="13"/>
       <c r="G152" s="13"/>
       <c r="H152" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I152" s="13"/>
       <c r="J152" s="13"/>
@@ -17882,7 +17957,7 @@
       </c>
       <c r="G164" s="13"/>
       <c r="H164" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I164" s="13"/>
       <c r="J164" s="13"/>
@@ -18005,7 +18080,7 @@
       <c r="F167" s="13"/>
       <c r="G167" s="13"/>
       <c r="H167" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I167" s="13"/>
       <c r="J167" s="13"/>
@@ -18342,7 +18417,7 @@
       </c>
       <c r="G174" s="13"/>
       <c r="H174" s="13">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I174" s="13"/>
       <c r="J174" s="13"/>
@@ -18508,36 +18583,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="9">
+    <row r="178" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="17">
         <v>176</v>
       </c>
-      <c r="B178" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C178" s="9">
+      <c r="B178" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C178" s="17">
         <v>30.258914999999998</v>
       </c>
-      <c r="D178" s="9">
+      <c r="D178" s="17">
         <v>-91.321944722222213</v>
       </c>
-      <c r="F178" s="13"/>
-      <c r="G178" s="13"/>
-      <c r="H178" s="13"/>
-      <c r="I178" s="13"/>
-      <c r="J178" s="13"/>
-      <c r="K178" s="13"/>
-      <c r="L178" s="13"/>
-      <c r="M178" s="13">
+      <c r="F178" s="19">
+        <v>0</v>
+      </c>
+      <c r="G178" s="19">
+        <v>0</v>
+      </c>
+      <c r="H178" s="19">
         <v>1</v>
       </c>
-      <c r="N178" s="13"/>
-      <c r="O178" s="13"/>
-      <c r="P178" s="13"/>
-      <c r="Q178" s="13"/>
-      <c r="R178" s="13"/>
-      <c r="S178" s="13"/>
-      <c r="T178" s="13"/>
+      <c r="I178" s="19">
+        <v>0</v>
+      </c>
+      <c r="J178" s="19">
+        <v>0</v>
+      </c>
+      <c r="K178" s="19">
+        <v>0</v>
+      </c>
+      <c r="L178" s="19">
+        <v>0</v>
+      </c>
+      <c r="M178" s="19">
+        <v>1</v>
+      </c>
+      <c r="N178" s="19">
+        <v>0</v>
+      </c>
+      <c r="O178" s="19">
+        <v>0</v>
+      </c>
+      <c r="P178" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q178" s="19">
+        <v>0</v>
+      </c>
+      <c r="R178" s="19">
+        <v>0</v>
+      </c>
+      <c r="S178" s="19">
+        <v>0</v>
+      </c>
+      <c r="T178" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A179">
@@ -18801,7 +18904,9 @@
       </c>
       <c r="F184" s="13"/>
       <c r="G184" s="13"/>
-      <c r="H184" s="13"/>
+      <c r="H184" s="13">
+        <v>1</v>
+      </c>
       <c r="I184" s="13"/>
       <c r="J184" s="13"/>
       <c r="K184" s="13"/>
@@ -19015,7 +19120,7 @@
       <c r="F189" s="13"/>
       <c r="G189" s="13"/>
       <c r="H189" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I189" s="13"/>
       <c r="J189" s="13"/>
@@ -19046,7 +19151,7 @@
       <c r="F190" s="13"/>
       <c r="G190" s="13"/>
       <c r="H190" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I190" s="13"/>
       <c r="J190" s="13">
@@ -19788,19 +19893,67 @@
       <c r="D206" s="9">
         <v>-90.237831999999997</v>
       </c>
-    </row>
-    <row r="207" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="9">
+      <c r="Q206" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="17">
         <v>205</v>
       </c>
-      <c r="B207" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C207" s="9">
+      <c r="B207" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="17">
         <v>30.020377700000001</v>
       </c>
-      <c r="D207" s="9">
+      <c r="D207" s="17">
         <v>-90.142554000000004</v>
+      </c>
+      <c r="F207" s="17">
+        <v>11</v>
+      </c>
+      <c r="G207" s="17">
+        <v>0</v>
+      </c>
+      <c r="H207" s="17">
+        <v>0</v>
+      </c>
+      <c r="I207" s="17">
+        <v>0</v>
+      </c>
+      <c r="J207" s="17">
+        <v>0</v>
+      </c>
+      <c r="K207" s="17">
+        <v>0</v>
+      </c>
+      <c r="L207" s="17">
+        <v>0</v>
+      </c>
+      <c r="M207" s="17">
+        <v>0</v>
+      </c>
+      <c r="N207" s="17">
+        <v>2</v>
+      </c>
+      <c r="O207" s="17">
+        <v>0</v>
+      </c>
+      <c r="P207" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q207" s="17">
+        <v>9</v>
+      </c>
+      <c r="R207" s="17">
+        <v>0</v>
+      </c>
+      <c r="S207" s="17">
+        <v>0</v>
+      </c>
+      <c r="T207" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -19817,222 +19970,318 @@
         <v>-90.734886500000002</v>
       </c>
     </row>
-    <row r="209" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A209" s="19">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A209">
         <v>207</v>
       </c>
-      <c r="B209" s="20" t="s">
+      <c r="B209" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C209" s="19">
+      <c r="C209">
         <v>30.101043000000001</v>
       </c>
-      <c r="D209" s="19">
+      <c r="D209">
         <v>-90.736847699999998</v>
       </c>
-      <c r="F209" s="19">
-        <v>0</v>
-      </c>
-      <c r="G209" s="19">
-        <v>0</v>
-      </c>
-      <c r="H209" s="19">
-        <v>0</v>
-      </c>
-      <c r="I209" s="19">
-        <v>0</v>
-      </c>
-      <c r="J209" s="19">
-        <v>0</v>
-      </c>
-      <c r="K209" s="19">
-        <v>0</v>
-      </c>
-      <c r="L209" s="19">
-        <v>0</v>
-      </c>
-      <c r="M209" s="19">
-        <v>0</v>
-      </c>
-      <c r="N209" s="19">
-        <v>0</v>
-      </c>
-      <c r="O209" s="19">
-        <v>0</v>
-      </c>
-      <c r="P209" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q209" s="19">
-        <v>0</v>
-      </c>
-      <c r="R209" s="19">
-        <v>0</v>
-      </c>
-      <c r="S209" s="19">
-        <v>0</v>
-      </c>
-      <c r="T209" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="16">
+      <c r="F209">
+        <v>0</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+      <c r="I209">
+        <v>0</v>
+      </c>
+      <c r="J209">
+        <v>0</v>
+      </c>
+      <c r="K209">
+        <v>0</v>
+      </c>
+      <c r="L209">
+        <v>0</v>
+      </c>
+      <c r="M209">
+        <v>0</v>
+      </c>
+      <c r="N209">
+        <v>0</v>
+      </c>
+      <c r="O209">
+        <v>0</v>
+      </c>
+      <c r="P209">
+        <v>0</v>
+      </c>
+      <c r="Q209">
+        <v>0</v>
+      </c>
+      <c r="R209">
+        <v>0</v>
+      </c>
+      <c r="S209">
+        <v>0</v>
+      </c>
+      <c r="T209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="9">
         <v>208</v>
       </c>
-      <c r="B210" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C210" s="16">
+      <c r="B210" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210" s="9">
         <v>29.598918333333334</v>
       </c>
-      <c r="D210" s="16">
+      <c r="D210" s="9">
         <v>-90.710750000000004</v>
       </c>
-    </row>
-    <row r="211" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="16">
+      <c r="F210" s="9">
+        <v>2</v>
+      </c>
+      <c r="M210" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="17">
         <v>209</v>
       </c>
-      <c r="B211" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C211" s="16">
+      <c r="B211" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211" s="17">
         <v>29.578356111111113</v>
       </c>
-      <c r="D211" s="16">
+      <c r="D211" s="17">
         <v>-90.721383055555563</v>
       </c>
-    </row>
-    <row r="212" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="16">
+      <c r="F211" s="17">
+        <v>0</v>
+      </c>
+      <c r="G211" s="17">
+        <v>0</v>
+      </c>
+      <c r="H211" s="17">
+        <v>1</v>
+      </c>
+      <c r="I211" s="17">
+        <v>0</v>
+      </c>
+      <c r="J211" s="17">
+        <v>0</v>
+      </c>
+      <c r="K211" s="17">
+        <v>0</v>
+      </c>
+      <c r="L211" s="17">
+        <v>0</v>
+      </c>
+      <c r="M211" s="17">
+        <v>3</v>
+      </c>
+      <c r="N211" s="17">
+        <v>0</v>
+      </c>
+      <c r="O211" s="17">
+        <v>0</v>
+      </c>
+      <c r="P211" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q211" s="17">
+        <v>0</v>
+      </c>
+      <c r="R211" s="17">
+        <v>0</v>
+      </c>
+      <c r="S211" s="17">
+        <v>0</v>
+      </c>
+      <c r="T211" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="17">
         <v>210</v>
       </c>
-      <c r="B212" s="17" t="s">
+      <c r="B212" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C212" s="16">
+      <c r="C212" s="17">
         <v>29.586098888888888</v>
       </c>
-      <c r="D212" s="16">
+      <c r="D212" s="17">
         <v>-90.752934444444449</v>
       </c>
-      <c r="F212" s="16">
-        <v>0</v>
-      </c>
-      <c r="G212" s="16">
-        <v>0</v>
-      </c>
-      <c r="H212" s="16">
-        <v>0</v>
-      </c>
-      <c r="I212" s="16">
-        <v>0</v>
-      </c>
-      <c r="J212" s="16">
-        <v>0</v>
-      </c>
-      <c r="K212" s="16">
-        <v>0</v>
-      </c>
-      <c r="L212" s="16">
-        <v>0</v>
-      </c>
-      <c r="M212" s="16">
-        <v>0</v>
-      </c>
-      <c r="N212" s="16">
-        <v>0</v>
-      </c>
-      <c r="O212" s="16">
-        <v>0</v>
-      </c>
-      <c r="P212" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q212" s="16">
-        <v>0</v>
-      </c>
-      <c r="R212" s="16">
-        <v>0</v>
-      </c>
-      <c r="S212" s="16">
-        <v>0</v>
-      </c>
-      <c r="T212" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="16">
+      <c r="F212" s="17">
+        <v>0</v>
+      </c>
+      <c r="G212" s="17">
+        <v>0</v>
+      </c>
+      <c r="H212" s="17">
+        <v>0</v>
+      </c>
+      <c r="I212" s="17">
+        <v>0</v>
+      </c>
+      <c r="J212" s="17">
+        <v>0</v>
+      </c>
+      <c r="K212" s="17">
+        <v>0</v>
+      </c>
+      <c r="L212" s="17">
+        <v>0</v>
+      </c>
+      <c r="M212" s="17">
+        <v>0</v>
+      </c>
+      <c r="N212" s="17">
+        <v>0</v>
+      </c>
+      <c r="O212" s="17">
+        <v>0</v>
+      </c>
+      <c r="P212" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q212" s="17">
+        <v>0</v>
+      </c>
+      <c r="R212" s="17">
+        <v>0</v>
+      </c>
+      <c r="S212" s="17">
+        <v>0</v>
+      </c>
+      <c r="T212" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="17">
         <v>211</v>
       </c>
-      <c r="B213" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C213" s="16">
+      <c r="B213" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213" s="17">
         <v>29.561021111111113</v>
       </c>
-      <c r="D213" s="16">
+      <c r="D213" s="17">
         <v>-90.791579722222224</v>
       </c>
-    </row>
-    <row r="214" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A214" s="16">
+      <c r="F213" s="17">
+        <v>0</v>
+      </c>
+      <c r="G213" s="17">
+        <v>0</v>
+      </c>
+      <c r="H213" s="17">
+        <v>8</v>
+      </c>
+      <c r="I213" s="17">
+        <v>0</v>
+      </c>
+      <c r="J213" s="17">
+        <v>0</v>
+      </c>
+      <c r="K213" s="17">
+        <v>0</v>
+      </c>
+      <c r="L213" s="17">
+        <v>0</v>
+      </c>
+      <c r="M213" s="17">
+        <v>4</v>
+      </c>
+      <c r="N213" s="17">
+        <v>0</v>
+      </c>
+      <c r="O213" s="17">
+        <v>0</v>
+      </c>
+      <c r="P213" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q213" s="17">
+        <v>0</v>
+      </c>
+      <c r="R213" s="17">
+        <v>0</v>
+      </c>
+      <c r="S213" s="17">
+        <v>0</v>
+      </c>
+      <c r="T213" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="17">
         <v>212</v>
       </c>
-      <c r="B214" s="17" t="s">
+      <c r="B214" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C214" s="16">
+      <c r="C214" s="17">
         <v>29.54808666666667</v>
       </c>
-      <c r="D214" s="16">
+      <c r="D214" s="17">
         <v>-90.79129555555555</v>
       </c>
-      <c r="F214" s="16">
-        <v>0</v>
-      </c>
-      <c r="G214" s="16">
-        <v>0</v>
-      </c>
-      <c r="H214" s="16">
-        <v>0</v>
-      </c>
-      <c r="I214" s="16">
-        <v>0</v>
-      </c>
-      <c r="J214" s="16">
-        <v>0</v>
-      </c>
-      <c r="K214" s="16">
-        <v>0</v>
-      </c>
-      <c r="L214" s="16">
-        <v>0</v>
-      </c>
-      <c r="M214" s="16">
-        <v>0</v>
-      </c>
-      <c r="N214" s="16">
-        <v>0</v>
-      </c>
-      <c r="O214" s="16">
-        <v>0</v>
-      </c>
-      <c r="P214" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q214" s="16">
-        <v>0</v>
-      </c>
-      <c r="R214" s="16">
-        <v>0</v>
-      </c>
-      <c r="S214" s="16">
-        <v>0</v>
-      </c>
-      <c r="T214" s="16">
+      <c r="F214" s="17">
+        <v>0</v>
+      </c>
+      <c r="G214" s="17">
+        <v>0</v>
+      </c>
+      <c r="H214" s="17">
+        <v>0</v>
+      </c>
+      <c r="I214" s="17">
+        <v>0</v>
+      </c>
+      <c r="J214" s="17">
+        <v>0</v>
+      </c>
+      <c r="K214" s="17">
+        <v>0</v>
+      </c>
+      <c r="L214" s="17">
+        <v>0</v>
+      </c>
+      <c r="M214" s="17">
+        <v>0</v>
+      </c>
+      <c r="N214" s="17">
+        <v>0</v>
+      </c>
+      <c r="O214" s="17">
+        <v>0</v>
+      </c>
+      <c r="P214" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q214" s="17">
+        <v>0</v>
+      </c>
+      <c r="R214" s="17">
+        <v>0</v>
+      </c>
+      <c r="S214" s="17">
+        <v>0</v>
+      </c>
+      <c r="T214" s="17">
         <v>0</v>
       </c>
     </row>
@@ -20044,10 +20293,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D35" sqref="A35:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20517,6 +20766,34 @@
         <v>-91.191599722222222</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="17">
+        <v>205</v>
+      </c>
+      <c r="B34" s="17">
+        <v>30.020377700000001</v>
+      </c>
+      <c r="C34" s="17">
+        <v>-90.142554000000004</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="17">
+        <v>208</v>
+      </c>
+      <c r="B35" s="17">
+        <v>29.598918333333334</v>
+      </c>
+      <c r="C35" s="17">
+        <v>-90.710750000000004</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -20826,10 +21103,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21698,56 +21975,56 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="17">
+        <v>176</v>
+      </c>
+      <c r="B62" s="17">
+        <v>30.258914999999998</v>
+      </c>
+      <c r="C62" s="17">
+        <v>-91.321944722222213</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
         <v>178</v>
       </c>
-      <c r="B62">
+      <c r="B63">
         <v>30.399977777777778</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <v>-91.512002222222222</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
-        <v>185</v>
-      </c>
-      <c r="B63">
-        <v>32.171768055555553</v>
-      </c>
-      <c r="C63">
-        <v>-92.992765833333337</v>
-      </c>
       <c r="D63" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
-        <v>186</v>
-      </c>
-      <c r="B64">
-        <v>32.314416666666666</v>
-      </c>
-      <c r="C64">
-        <v>-93.151305555555567</v>
-      </c>
-      <c r="D64" s="3" t="s">
+      <c r="A64" s="17">
+        <v>182</v>
+      </c>
+      <c r="B64" s="17">
+        <v>32.312416666666664</v>
+      </c>
+      <c r="C64" s="17">
+        <v>-92.443666666666672</v>
+      </c>
+      <c r="D64" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B65">
-        <v>32.597631666666672</v>
+        <v>32.171768055555553</v>
       </c>
       <c r="C65">
-        <v>-93.333229722222214</v>
+        <v>-92.992765833333337</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>3</v>
@@ -21755,13 +22032,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B66">
-        <v>32.323081666666667</v>
+        <v>32.314416666666666</v>
       </c>
       <c r="C66">
-        <v>-93.41498555555556</v>
+        <v>-93.151305555555567</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>3</v>
@@ -21769,15 +22046,71 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
+        <v>187</v>
+      </c>
+      <c r="B67">
+        <v>32.597631666666672</v>
+      </c>
+      <c r="C67">
+        <v>-93.333229722222214</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>188</v>
+      </c>
+      <c r="B68">
+        <v>32.323081666666667</v>
+      </c>
+      <c r="C68">
+        <v>-93.41498555555556</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
         <v>202</v>
       </c>
-      <c r="B67" s="18">
+      <c r="B69" s="16">
         <v>30.412583999999999</v>
       </c>
-      <c r="C67" s="18">
+      <c r="C69" s="16">
         <v>-90.974874999999997</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D69" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="17">
+        <v>209</v>
+      </c>
+      <c r="B70" s="17">
+        <v>29.578356111111113</v>
+      </c>
+      <c r="C70" s="17">
+        <v>-90.721383055555563</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="17">
+        <v>211</v>
+      </c>
+      <c r="B71" s="17">
+        <v>29.561021111111113</v>
+      </c>
+      <c r="C71" s="17">
+        <v>-90.791579722222224</v>
+      </c>
+      <c r="D71" s="18" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added sites from recent sponge (Friday, March 3rd, and Sunday, March 5th) map of all sites.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/new_spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36942384-226F-DB43-8AB3-A6DD66082AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB2CAF9-680F-1942-BC6C-AB8B8AABE2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -188,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +198,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
@@ -261,11 +267,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L217"/>
+  <dimension ref="A1:L231"/>
   <sheetViews>
-    <sheetView topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="E217" sqref="E217"/>
+    <sheetView topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="I218" sqref="I218:I231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4648,7 +4653,7 @@
         <v>15.49</v>
       </c>
       <c r="E135" s="3">
-        <f t="shared" ref="E135:E217" si="18">B135+C135/60+D135/3600</f>
+        <f t="shared" ref="E135:E231" si="18">B135+C135/60+D135/3600</f>
         <v>30.370969444444444</v>
       </c>
       <c r="F135" s="1">
@@ -4661,7 +4666,7 @@
         <v>31.54</v>
       </c>
       <c r="I135">
-        <f t="shared" ref="I135:I217" si="19">-F135-G135/60-H135/3600</f>
+        <f t="shared" ref="I135:I231" si="19">-F135-G135/60-H135/3600</f>
         <v>-91.625427777777773</v>
       </c>
     </row>
@@ -7205,6 +7210,440 @@
       <c r="I217">
         <f t="shared" si="19"/>
         <v>-90.79129555555555</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>213</v>
+      </c>
+      <c r="B218" s="1">
+        <v>30</v>
+      </c>
+      <c r="C218">
+        <v>32</v>
+      </c>
+      <c r="D218">
+        <v>28.298999999999999</v>
+      </c>
+      <c r="E218" s="3">
+        <f t="shared" si="18"/>
+        <v>30.541194166666667</v>
+      </c>
+      <c r="F218" s="1">
+        <v>91</v>
+      </c>
+      <c r="G218">
+        <v>47</v>
+      </c>
+      <c r="H218">
+        <v>25.370999999999999</v>
+      </c>
+      <c r="I218">
+        <f t="shared" si="19"/>
+        <v>-91.79038083333333</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>214</v>
+      </c>
+      <c r="B219" s="1">
+        <v>30</v>
+      </c>
+      <c r="C219">
+        <v>32</v>
+      </c>
+      <c r="D219">
+        <v>59.070999999999998</v>
+      </c>
+      <c r="E219" s="3">
+        <f t="shared" si="18"/>
+        <v>30.549741944444445</v>
+      </c>
+      <c r="F219" s="1">
+        <v>91</v>
+      </c>
+      <c r="G219">
+        <v>52</v>
+      </c>
+      <c r="H219">
+        <v>23.356999999999999</v>
+      </c>
+      <c r="I219">
+        <f t="shared" si="19"/>
+        <v>-91.87315472222221</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>215</v>
+      </c>
+      <c r="B220" s="1">
+        <v>30</v>
+      </c>
+      <c r="C220">
+        <v>25</v>
+      </c>
+      <c r="D220">
+        <v>54.75</v>
+      </c>
+      <c r="E220" s="3">
+        <f t="shared" si="18"/>
+        <v>30.431875000000002</v>
+      </c>
+      <c r="F220" s="1">
+        <v>91</v>
+      </c>
+      <c r="G220">
+        <v>52</v>
+      </c>
+      <c r="H220">
+        <v>31.52</v>
+      </c>
+      <c r="I220">
+        <f t="shared" si="19"/>
+        <v>-91.875422222222213</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>216</v>
+      </c>
+      <c r="B221" s="1">
+        <v>30</v>
+      </c>
+      <c r="C221">
+        <v>30</v>
+      </c>
+      <c r="D221">
+        <v>9.3670000000000009</v>
+      </c>
+      <c r="E221" s="3">
+        <f t="shared" si="18"/>
+        <v>30.502601944444443</v>
+      </c>
+      <c r="F221" s="1">
+        <v>92</v>
+      </c>
+      <c r="G221">
+        <v>54</v>
+      </c>
+      <c r="H221">
+        <v>55.212000000000003</v>
+      </c>
+      <c r="I221">
+        <f t="shared" si="19"/>
+        <v>-92.915336666666676</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>217</v>
+      </c>
+      <c r="B222" s="1">
+        <v>30</v>
+      </c>
+      <c r="C222">
+        <v>30</v>
+      </c>
+      <c r="D222">
+        <v>42.344000000000001</v>
+      </c>
+      <c r="E222" s="3">
+        <f t="shared" si="18"/>
+        <v>30.511762222222224</v>
+      </c>
+      <c r="F222" s="1">
+        <v>93</v>
+      </c>
+      <c r="G222">
+        <v>13</v>
+      </c>
+      <c r="H222">
+        <v>52.822000000000003</v>
+      </c>
+      <c r="I222">
+        <f t="shared" si="19"/>
+        <v>-93.231339444444444</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>218</v>
+      </c>
+      <c r="B223" s="1">
+        <v>31</v>
+      </c>
+      <c r="C223">
+        <v>12</v>
+      </c>
+      <c r="D223">
+        <v>25.378</v>
+      </c>
+      <c r="E223" s="3">
+        <f t="shared" si="18"/>
+        <v>31.207049444444444</v>
+      </c>
+      <c r="F223" s="1">
+        <v>93</v>
+      </c>
+      <c r="G223">
+        <v>34</v>
+      </c>
+      <c r="H223">
+        <v>45.165999999999997</v>
+      </c>
+      <c r="I223">
+        <f t="shared" si="19"/>
+        <v>-93.579212777777769</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>219</v>
+      </c>
+      <c r="B224" s="1">
+        <v>31</v>
+      </c>
+      <c r="C224">
+        <v>12</v>
+      </c>
+      <c r="D224">
+        <v>15.519</v>
+      </c>
+      <c r="E224" s="3">
+        <f t="shared" si="18"/>
+        <v>31.204310833333334</v>
+      </c>
+      <c r="F224" s="1">
+        <v>93</v>
+      </c>
+      <c r="G224">
+        <v>32</v>
+      </c>
+      <c r="H224">
+        <v>41.164999999999999</v>
+      </c>
+      <c r="I224">
+        <f t="shared" si="19"/>
+        <v>-93.544768055555551</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>220</v>
+      </c>
+      <c r="B225" s="1">
+        <v>31</v>
+      </c>
+      <c r="C225">
+        <v>23</v>
+      </c>
+      <c r="D225">
+        <v>49.433</v>
+      </c>
+      <c r="E225" s="3">
+        <f t="shared" si="18"/>
+        <v>31.397064722222222</v>
+      </c>
+      <c r="F225" s="1">
+        <v>92</v>
+      </c>
+      <c r="G225">
+        <v>40</v>
+      </c>
+      <c r="H225">
+        <v>20.541</v>
+      </c>
+      <c r="I225">
+        <f t="shared" si="19"/>
+        <v>-92.672372500000009</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>221</v>
+      </c>
+      <c r="B226" s="1">
+        <v>31</v>
+      </c>
+      <c r="C226">
+        <v>19</v>
+      </c>
+      <c r="D226">
+        <v>54.631999999999998</v>
+      </c>
+      <c r="E226" s="3">
+        <f t="shared" si="18"/>
+        <v>31.331842222222221</v>
+      </c>
+      <c r="F226" s="1">
+        <v>92</v>
+      </c>
+      <c r="G226">
+        <v>26</v>
+      </c>
+      <c r="H226">
+        <v>39.280999999999999</v>
+      </c>
+      <c r="I226">
+        <f t="shared" si="19"/>
+        <v>-92.444244722222223</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>222</v>
+      </c>
+      <c r="B227" s="1">
+        <v>31</v>
+      </c>
+      <c r="C227">
+        <v>19</v>
+      </c>
+      <c r="D227">
+        <v>13.858000000000001</v>
+      </c>
+      <c r="E227" s="3">
+        <f t="shared" si="18"/>
+        <v>31.320516111111111</v>
+      </c>
+      <c r="F227" s="1">
+        <v>92</v>
+      </c>
+      <c r="G227">
+        <v>26</v>
+      </c>
+      <c r="H227">
+        <v>54.426000000000002</v>
+      </c>
+      <c r="I227">
+        <f t="shared" si="19"/>
+        <v>-92.448451666666671</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>223</v>
+      </c>
+      <c r="B228" s="1">
+        <v>31</v>
+      </c>
+      <c r="C228">
+        <v>18</v>
+      </c>
+      <c r="D228">
+        <v>53.034999999999997</v>
+      </c>
+      <c r="E228" s="3">
+        <f t="shared" si="18"/>
+        <v>31.314731944444446</v>
+      </c>
+      <c r="F228" s="1">
+        <v>92</v>
+      </c>
+      <c r="G228">
+        <v>26</v>
+      </c>
+      <c r="H228">
+        <v>36.701999999999998</v>
+      </c>
+      <c r="I228">
+        <f t="shared" si="19"/>
+        <v>-92.443528333333333</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>224</v>
+      </c>
+      <c r="B229" s="1">
+        <v>31</v>
+      </c>
+      <c r="C229">
+        <v>6</v>
+      </c>
+      <c r="D229">
+        <v>40.85</v>
+      </c>
+      <c r="E229" s="3">
+        <f t="shared" si="18"/>
+        <v>31.111347222222225</v>
+      </c>
+      <c r="F229" s="1">
+        <v>92</v>
+      </c>
+      <c r="G229">
+        <v>28</v>
+      </c>
+      <c r="H229">
+        <v>10.032</v>
+      </c>
+      <c r="I229">
+        <f t="shared" si="19"/>
+        <v>-92.469453333333334</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>225</v>
+      </c>
+      <c r="B230" s="1">
+        <v>29</v>
+      </c>
+      <c r="C230">
+        <v>55</v>
+      </c>
+      <c r="D230">
+        <v>59.21</v>
+      </c>
+      <c r="E230" s="3">
+        <f t="shared" si="18"/>
+        <v>29.93311388888889</v>
+      </c>
+      <c r="F230" s="1">
+        <v>93</v>
+      </c>
+      <c r="G230">
+        <v>4</v>
+      </c>
+      <c r="H230">
+        <v>45.354999999999997</v>
+      </c>
+      <c r="I230">
+        <f t="shared" si="19"/>
+        <v>-93.079265277777779</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>226</v>
+      </c>
+      <c r="B231" s="1">
+        <v>29</v>
+      </c>
+      <c r="C231">
+        <v>44</v>
+      </c>
+      <c r="D231">
+        <v>47.088000000000001</v>
+      </c>
+      <c r="E231" s="3">
+        <f t="shared" si="18"/>
+        <v>29.746413333333333</v>
+      </c>
+      <c r="F231" s="1">
+        <v>92</v>
+      </c>
+      <c r="G231">
+        <v>19</v>
+      </c>
+      <c r="H231">
+        <v>29.995999999999999</v>
+      </c>
+      <c r="I231">
+        <f t="shared" si="19"/>
+        <v>-92.324998888888885</v>
       </c>
     </row>
   </sheetData>
@@ -8246,44 +8685,44 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="17">
+      <c r="A74">
         <v>208</v>
       </c>
-      <c r="B74" s="17">
+      <c r="B74">
         <v>29.598918333333334</v>
       </c>
-      <c r="C74" s="17">
+      <c r="C74">
         <v>-90.710750000000004</v>
       </c>
-      <c r="D74" s="18" t="s">
+      <c r="D74" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="17">
+      <c r="A75">
         <v>209</v>
       </c>
-      <c r="B75" s="17">
+      <c r="B75">
         <v>29.578356111111113</v>
       </c>
-      <c r="C75" s="17">
+      <c r="C75">
         <v>-90.721383055555563</v>
       </c>
-      <c r="D75" s="18" t="s">
+      <c r="D75" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="17">
+      <c r="A76">
         <v>211</v>
       </c>
-      <c r="B76" s="17">
+      <c r="B76">
         <v>29.561021111111113</v>
       </c>
-      <c r="C76" s="17">
+      <c r="C76">
         <v>-90.791579722222224</v>
       </c>
-      <c r="D76" s="18" t="s">
+      <c r="D76" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8432,16 +8871,16 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="17">
+      <c r="A10">
         <v>205</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10">
         <v>30.020377700000001</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10">
         <v>-90.142554000000004</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8867,30 +9306,30 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="A6">
         <v>204</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6">
         <v>30.043209000000001</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6">
         <v>-90.237831999999997</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
+      <c r="A7">
         <v>205</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7">
         <v>30.020377700000001</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7">
         <v>-90.142554000000004</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9014,11 +9453,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U214"/>
+  <dimension ref="A1:U228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A213" sqref="A213:D213"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O234" sqref="O234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18583,62 +19022,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="17">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A178">
         <v>176</v>
       </c>
-      <c r="B178" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C178" s="17">
+      <c r="B178" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C178">
         <v>30.258914999999998</v>
       </c>
-      <c r="D178" s="17">
+      <c r="D178">
         <v>-91.321944722222213</v>
       </c>
-      <c r="F178" s="19">
-        <v>0</v>
-      </c>
-      <c r="G178" s="19">
-        <v>0</v>
-      </c>
-      <c r="H178" s="19">
+      <c r="F178" s="10">
+        <v>0</v>
+      </c>
+      <c r="G178" s="10">
+        <v>0</v>
+      </c>
+      <c r="H178" s="10">
         <v>1</v>
       </c>
-      <c r="I178" s="19">
-        <v>0</v>
-      </c>
-      <c r="J178" s="19">
-        <v>0</v>
-      </c>
-      <c r="K178" s="19">
-        <v>0</v>
-      </c>
-      <c r="L178" s="19">
-        <v>0</v>
-      </c>
-      <c r="M178" s="19">
+      <c r="I178" s="10">
+        <v>0</v>
+      </c>
+      <c r="J178" s="10">
+        <v>0</v>
+      </c>
+      <c r="K178" s="10">
+        <v>0</v>
+      </c>
+      <c r="L178" s="10">
+        <v>0</v>
+      </c>
+      <c r="M178" s="10">
         <v>1</v>
       </c>
-      <c r="N178" s="19">
-        <v>0</v>
-      </c>
-      <c r="O178" s="19">
-        <v>0</v>
-      </c>
-      <c r="P178" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q178" s="19">
-        <v>0</v>
-      </c>
-      <c r="R178" s="19">
-        <v>0</v>
-      </c>
-      <c r="S178" s="19">
-        <v>0</v>
-      </c>
-      <c r="T178" s="19">
+      <c r="N178" s="10">
+        <v>0</v>
+      </c>
+      <c r="O178" s="10">
+        <v>0</v>
+      </c>
+      <c r="P178" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q178" s="10">
+        <v>0</v>
+      </c>
+      <c r="R178" s="10">
+        <v>0</v>
+      </c>
+      <c r="S178" s="10">
+        <v>0</v>
+      </c>
+      <c r="T178" s="10">
         <v>0</v>
       </c>
     </row>
@@ -19897,62 +20336,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="17">
+    <row r="207" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A207">
         <v>205</v>
       </c>
-      <c r="B207" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C207" s="17">
+      <c r="B207" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207">
         <v>30.020377700000001</v>
       </c>
-      <c r="D207" s="17">
+      <c r="D207">
         <v>-90.142554000000004</v>
       </c>
-      <c r="F207" s="17">
+      <c r="F207">
         <v>11</v>
       </c>
-      <c r="G207" s="17">
-        <v>0</v>
-      </c>
-      <c r="H207" s="17">
-        <v>0</v>
-      </c>
-      <c r="I207" s="17">
-        <v>0</v>
-      </c>
-      <c r="J207" s="17">
-        <v>0</v>
-      </c>
-      <c r="K207" s="17">
-        <v>0</v>
-      </c>
-      <c r="L207" s="17">
-        <v>0</v>
-      </c>
-      <c r="M207" s="17">
-        <v>0</v>
-      </c>
-      <c r="N207" s="17">
+      <c r="G207">
+        <v>0</v>
+      </c>
+      <c r="H207">
+        <v>0</v>
+      </c>
+      <c r="I207">
+        <v>0</v>
+      </c>
+      <c r="J207">
+        <v>0</v>
+      </c>
+      <c r="K207">
+        <v>0</v>
+      </c>
+      <c r="L207">
+        <v>0</v>
+      </c>
+      <c r="M207">
+        <v>0</v>
+      </c>
+      <c r="N207">
         <v>2</v>
       </c>
-      <c r="O207" s="17">
-        <v>0</v>
-      </c>
-      <c r="P207" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q207" s="17">
+      <c r="O207">
+        <v>0</v>
+      </c>
+      <c r="P207">
+        <v>0</v>
+      </c>
+      <c r="Q207">
         <v>9</v>
       </c>
-      <c r="R207" s="17">
-        <v>0</v>
-      </c>
-      <c r="S207" s="17">
-        <v>0</v>
-      </c>
-      <c r="T207" s="17">
+      <c r="R207">
+        <v>0</v>
+      </c>
+      <c r="S207">
+        <v>0</v>
+      </c>
+      <c r="T207">
         <v>0</v>
       </c>
     </row>
@@ -20049,240 +20488,796 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="17">
+    <row r="211" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A211">
         <v>209</v>
       </c>
-      <c r="B211" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C211" s="17">
+      <c r="B211" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211">
         <v>29.578356111111113</v>
       </c>
-      <c r="D211" s="17">
+      <c r="D211">
         <v>-90.721383055555563</v>
       </c>
-      <c r="F211" s="17">
-        <v>0</v>
-      </c>
-      <c r="G211" s="17">
-        <v>0</v>
-      </c>
-      <c r="H211" s="17">
+      <c r="F211">
+        <v>0</v>
+      </c>
+      <c r="G211">
+        <v>0</v>
+      </c>
+      <c r="H211">
         <v>1</v>
       </c>
-      <c r="I211" s="17">
-        <v>0</v>
-      </c>
-      <c r="J211" s="17">
-        <v>0</v>
-      </c>
-      <c r="K211" s="17">
-        <v>0</v>
-      </c>
-      <c r="L211" s="17">
-        <v>0</v>
-      </c>
-      <c r="M211" s="17">
-        <v>3</v>
-      </c>
-      <c r="N211" s="17">
-        <v>0</v>
-      </c>
-      <c r="O211" s="17">
-        <v>0</v>
-      </c>
-      <c r="P211" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q211" s="17">
-        <v>0</v>
-      </c>
-      <c r="R211" s="17">
-        <v>0</v>
-      </c>
-      <c r="S211" s="17">
-        <v>0</v>
-      </c>
-      <c r="T211" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="17">
+      <c r="I211">
+        <v>0</v>
+      </c>
+      <c r="J211">
+        <v>0</v>
+      </c>
+      <c r="K211">
+        <v>0</v>
+      </c>
+      <c r="L211">
+        <v>0</v>
+      </c>
+      <c r="M211">
+        <v>3</v>
+      </c>
+      <c r="N211">
+        <v>0</v>
+      </c>
+      <c r="O211">
+        <v>0</v>
+      </c>
+      <c r="P211">
+        <v>0</v>
+      </c>
+      <c r="Q211">
+        <v>0</v>
+      </c>
+      <c r="R211">
+        <v>0</v>
+      </c>
+      <c r="S211">
+        <v>0</v>
+      </c>
+      <c r="T211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A212">
         <v>210</v>
       </c>
-      <c r="B212" s="18" t="s">
+      <c r="B212" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C212" s="17">
+      <c r="C212">
         <v>29.586098888888888</v>
       </c>
-      <c r="D212" s="17">
+      <c r="D212">
         <v>-90.752934444444449</v>
       </c>
-      <c r="F212" s="17">
-        <v>0</v>
-      </c>
-      <c r="G212" s="17">
-        <v>0</v>
-      </c>
-      <c r="H212" s="17">
-        <v>0</v>
-      </c>
-      <c r="I212" s="17">
-        <v>0</v>
-      </c>
-      <c r="J212" s="17">
-        <v>0</v>
-      </c>
-      <c r="K212" s="17">
-        <v>0</v>
-      </c>
-      <c r="L212" s="17">
-        <v>0</v>
-      </c>
-      <c r="M212" s="17">
-        <v>0</v>
-      </c>
-      <c r="N212" s="17">
-        <v>0</v>
-      </c>
-      <c r="O212" s="17">
-        <v>0</v>
-      </c>
-      <c r="P212" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q212" s="17">
-        <v>0</v>
-      </c>
-      <c r="R212" s="17">
-        <v>0</v>
-      </c>
-      <c r="S212" s="17">
-        <v>0</v>
-      </c>
-      <c r="T212" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="17">
+      <c r="F212">
+        <v>0</v>
+      </c>
+      <c r="G212">
+        <v>0</v>
+      </c>
+      <c r="H212">
+        <v>0</v>
+      </c>
+      <c r="I212">
+        <v>0</v>
+      </c>
+      <c r="J212">
+        <v>0</v>
+      </c>
+      <c r="K212">
+        <v>0</v>
+      </c>
+      <c r="L212">
+        <v>0</v>
+      </c>
+      <c r="M212">
+        <v>0</v>
+      </c>
+      <c r="N212">
+        <v>0</v>
+      </c>
+      <c r="O212">
+        <v>0</v>
+      </c>
+      <c r="P212">
+        <v>0</v>
+      </c>
+      <c r="Q212">
+        <v>0</v>
+      </c>
+      <c r="R212">
+        <v>0</v>
+      </c>
+      <c r="S212">
+        <v>0</v>
+      </c>
+      <c r="T212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A213">
         <v>211</v>
       </c>
-      <c r="B213" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C213" s="17">
+      <c r="B213" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213">
         <v>29.561021111111113</v>
       </c>
-      <c r="D213" s="17">
+      <c r="D213">
         <v>-90.791579722222224</v>
       </c>
-      <c r="F213" s="17">
-        <v>0</v>
-      </c>
-      <c r="G213" s="17">
-        <v>0</v>
-      </c>
-      <c r="H213" s="17">
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213">
+        <v>0</v>
+      </c>
+      <c r="H213">
         <v>8</v>
       </c>
-      <c r="I213" s="17">
-        <v>0</v>
-      </c>
-      <c r="J213" s="17">
-        <v>0</v>
-      </c>
-      <c r="K213" s="17">
-        <v>0</v>
-      </c>
-      <c r="L213" s="17">
-        <v>0</v>
-      </c>
-      <c r="M213" s="17">
+      <c r="I213">
+        <v>0</v>
+      </c>
+      <c r="J213">
+        <v>0</v>
+      </c>
+      <c r="K213">
+        <v>0</v>
+      </c>
+      <c r="L213">
+        <v>0</v>
+      </c>
+      <c r="M213">
         <v>4</v>
       </c>
-      <c r="N213" s="17">
-        <v>0</v>
-      </c>
-      <c r="O213" s="17">
-        <v>0</v>
-      </c>
-      <c r="P213" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q213" s="17">
-        <v>0</v>
-      </c>
-      <c r="R213" s="17">
-        <v>0</v>
-      </c>
-      <c r="S213" s="17">
-        <v>0</v>
-      </c>
-      <c r="T213" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A214" s="17">
+      <c r="N213">
+        <v>0</v>
+      </c>
+      <c r="O213">
+        <v>0</v>
+      </c>
+      <c r="P213">
+        <v>0</v>
+      </c>
+      <c r="Q213">
+        <v>0</v>
+      </c>
+      <c r="R213">
+        <v>0</v>
+      </c>
+      <c r="S213">
+        <v>0</v>
+      </c>
+      <c r="T213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A214">
         <v>212</v>
       </c>
-      <c r="B214" s="18" t="s">
+      <c r="B214" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C214" s="17">
+      <c r="C214">
         <v>29.54808666666667</v>
       </c>
-      <c r="D214" s="17">
+      <c r="D214">
         <v>-90.79129555555555</v>
       </c>
-      <c r="F214" s="17">
-        <v>0</v>
-      </c>
-      <c r="G214" s="17">
-        <v>0</v>
-      </c>
-      <c r="H214" s="17">
-        <v>0</v>
-      </c>
-      <c r="I214" s="17">
-        <v>0</v>
-      </c>
-      <c r="J214" s="17">
-        <v>0</v>
-      </c>
-      <c r="K214" s="17">
-        <v>0</v>
-      </c>
-      <c r="L214" s="17">
-        <v>0</v>
-      </c>
-      <c r="M214" s="17">
-        <v>0</v>
-      </c>
-      <c r="N214" s="17">
-        <v>0</v>
-      </c>
-      <c r="O214" s="17">
-        <v>0</v>
-      </c>
-      <c r="P214" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q214" s="17">
-        <v>0</v>
-      </c>
-      <c r="R214" s="17">
-        <v>0</v>
-      </c>
-      <c r="S214" s="17">
-        <v>0</v>
-      </c>
-      <c r="T214" s="17">
-        <v>0</v>
+      <c r="F214">
+        <v>0</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214">
+        <v>0</v>
+      </c>
+      <c r="I214">
+        <v>0</v>
+      </c>
+      <c r="J214">
+        <v>0</v>
+      </c>
+      <c r="K214">
+        <v>0</v>
+      </c>
+      <c r="L214">
+        <v>0</v>
+      </c>
+      <c r="M214">
+        <v>0</v>
+      </c>
+      <c r="N214">
+        <v>0</v>
+      </c>
+      <c r="O214">
+        <v>0</v>
+      </c>
+      <c r="P214">
+        <v>0</v>
+      </c>
+      <c r="Q214">
+        <v>0</v>
+      </c>
+      <c r="R214">
+        <v>0</v>
+      </c>
+      <c r="S214">
+        <v>0</v>
+      </c>
+      <c r="T214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="17">
+        <v>213</v>
+      </c>
+      <c r="B215" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C215" s="17">
+        <v>30.541194166666667</v>
+      </c>
+      <c r="D215" s="17">
+        <v>-91.79038083333333</v>
+      </c>
+    </row>
+    <row r="216" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="17">
+        <v>214</v>
+      </c>
+      <c r="B216" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C216" s="17">
+        <v>30.549741944444445</v>
+      </c>
+      <c r="D216" s="17">
+        <v>-91.87315472222221</v>
+      </c>
+    </row>
+    <row r="217" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="17">
+        <v>215</v>
+      </c>
+      <c r="B217" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C217" s="17">
+        <v>30.431875000000002</v>
+      </c>
+      <c r="D217" s="17">
+        <v>-91.875422222222213</v>
+      </c>
+    </row>
+    <row r="218" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="17">
+        <v>216</v>
+      </c>
+      <c r="B218" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C218" s="17">
+        <v>30.502601944444443</v>
+      </c>
+      <c r="D218" s="17">
+        <v>-92.915336666666676</v>
+      </c>
+      <c r="F218" s="17">
+        <v>0</v>
+      </c>
+      <c r="G218" s="17">
+        <v>0</v>
+      </c>
+      <c r="H218" s="17">
+        <v>0</v>
+      </c>
+      <c r="I218" s="17">
+        <v>0</v>
+      </c>
+      <c r="J218" s="17">
+        <v>0</v>
+      </c>
+      <c r="K218" s="17">
+        <v>0</v>
+      </c>
+      <c r="L218" s="17">
+        <v>0</v>
+      </c>
+      <c r="M218" s="17">
+        <v>0</v>
+      </c>
+      <c r="N218" s="17">
+        <v>0</v>
+      </c>
+      <c r="O218" s="17">
+        <v>0</v>
+      </c>
+      <c r="P218" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q218" s="17">
+        <v>0</v>
+      </c>
+      <c r="R218" s="17">
+        <v>0</v>
+      </c>
+      <c r="S218" s="17">
+        <v>0</v>
+      </c>
+      <c r="T218" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="17">
+        <v>217</v>
+      </c>
+      <c r="B219" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C219" s="17">
+        <v>30.511762222222224</v>
+      </c>
+      <c r="D219" s="17">
+        <v>-93.231339444444444</v>
+      </c>
+      <c r="F219" s="17">
+        <v>0</v>
+      </c>
+      <c r="G219" s="17">
+        <v>0</v>
+      </c>
+      <c r="H219" s="17">
+        <v>0</v>
+      </c>
+      <c r="I219" s="17">
+        <v>0</v>
+      </c>
+      <c r="J219" s="17">
+        <v>0</v>
+      </c>
+      <c r="K219" s="17">
+        <v>0</v>
+      </c>
+      <c r="L219" s="17">
+        <v>0</v>
+      </c>
+      <c r="M219" s="17">
+        <v>0</v>
+      </c>
+      <c r="N219" s="17">
+        <v>0</v>
+      </c>
+      <c r="O219" s="17">
+        <v>0</v>
+      </c>
+      <c r="P219" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q219" s="17">
+        <v>0</v>
+      </c>
+      <c r="R219" s="17">
+        <v>0</v>
+      </c>
+      <c r="S219" s="17">
+        <v>0</v>
+      </c>
+      <c r="T219" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="17">
+        <v>218</v>
+      </c>
+      <c r="B220" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C220" s="17">
+        <v>31.207049444444444</v>
+      </c>
+      <c r="D220" s="17">
+        <v>-93.579212777777769</v>
+      </c>
+      <c r="F220" s="17">
+        <v>0</v>
+      </c>
+      <c r="G220" s="17">
+        <v>0</v>
+      </c>
+      <c r="H220" s="17">
+        <v>0</v>
+      </c>
+      <c r="I220" s="17">
+        <v>0</v>
+      </c>
+      <c r="J220" s="17">
+        <v>0</v>
+      </c>
+      <c r="K220" s="17">
+        <v>0</v>
+      </c>
+      <c r="L220" s="17">
+        <v>0</v>
+      </c>
+      <c r="M220" s="17">
+        <v>0</v>
+      </c>
+      <c r="N220" s="17">
+        <v>0</v>
+      </c>
+      <c r="O220" s="17">
+        <v>0</v>
+      </c>
+      <c r="P220" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q220" s="17">
+        <v>0</v>
+      </c>
+      <c r="R220" s="17">
+        <v>0</v>
+      </c>
+      <c r="S220" s="17">
+        <v>0</v>
+      </c>
+      <c r="T220" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="17">
+        <v>219</v>
+      </c>
+      <c r="B221" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C221" s="17">
+        <v>31.204310833333334</v>
+      </c>
+      <c r="D221" s="17">
+        <v>-93.544768055555551</v>
+      </c>
+      <c r="F221" s="17">
+        <v>0</v>
+      </c>
+      <c r="G221" s="17">
+        <v>0</v>
+      </c>
+      <c r="H221" s="17">
+        <v>0</v>
+      </c>
+      <c r="I221" s="17">
+        <v>0</v>
+      </c>
+      <c r="J221" s="17">
+        <v>0</v>
+      </c>
+      <c r="K221" s="17">
+        <v>0</v>
+      </c>
+      <c r="L221" s="17">
+        <v>0</v>
+      </c>
+      <c r="M221" s="17">
+        <v>0</v>
+      </c>
+      <c r="N221" s="17">
+        <v>0</v>
+      </c>
+      <c r="O221" s="17">
+        <v>0</v>
+      </c>
+      <c r="P221" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q221" s="17">
+        <v>0</v>
+      </c>
+      <c r="R221" s="17">
+        <v>0</v>
+      </c>
+      <c r="S221" s="17">
+        <v>0</v>
+      </c>
+      <c r="T221" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="17">
+        <v>220</v>
+      </c>
+      <c r="B222" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C222" s="17">
+        <v>31.397064722222222</v>
+      </c>
+      <c r="D222" s="17">
+        <v>-92.672372500000009</v>
+      </c>
+      <c r="F222" s="17">
+        <v>0</v>
+      </c>
+      <c r="G222" s="17">
+        <v>0</v>
+      </c>
+      <c r="H222" s="17">
+        <v>0</v>
+      </c>
+      <c r="I222" s="17">
+        <v>0</v>
+      </c>
+      <c r="J222" s="17">
+        <v>0</v>
+      </c>
+      <c r="K222" s="17">
+        <v>0</v>
+      </c>
+      <c r="L222" s="17">
+        <v>0</v>
+      </c>
+      <c r="M222" s="17">
+        <v>0</v>
+      </c>
+      <c r="N222" s="17">
+        <v>0</v>
+      </c>
+      <c r="O222" s="17">
+        <v>0</v>
+      </c>
+      <c r="P222" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q222" s="17">
+        <v>0</v>
+      </c>
+      <c r="R222" s="17">
+        <v>0</v>
+      </c>
+      <c r="S222" s="17">
+        <v>0</v>
+      </c>
+      <c r="T222" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="17">
+        <v>221</v>
+      </c>
+      <c r="B223" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C223" s="17">
+        <v>31.331842222222221</v>
+      </c>
+      <c r="D223" s="17">
+        <v>-92.444244722222223</v>
+      </c>
+    </row>
+    <row r="224" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="17">
+        <v>222</v>
+      </c>
+      <c r="B224" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C224" s="17">
+        <v>31.320516111111111</v>
+      </c>
+      <c r="D224" s="17">
+        <v>-92.448451666666671</v>
+      </c>
+      <c r="F224" s="17">
+        <v>0</v>
+      </c>
+      <c r="G224" s="17">
+        <v>0</v>
+      </c>
+      <c r="H224" s="17">
+        <v>0</v>
+      </c>
+      <c r="I224" s="17">
+        <v>0</v>
+      </c>
+      <c r="J224" s="17">
+        <v>0</v>
+      </c>
+      <c r="K224" s="17">
+        <v>0</v>
+      </c>
+      <c r="L224" s="17">
+        <v>0</v>
+      </c>
+      <c r="M224" s="17">
+        <v>0</v>
+      </c>
+      <c r="N224" s="17">
+        <v>0</v>
+      </c>
+      <c r="O224" s="17">
+        <v>0</v>
+      </c>
+      <c r="P224" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q224" s="17">
+        <v>0</v>
+      </c>
+      <c r="R224" s="17">
+        <v>0</v>
+      </c>
+      <c r="S224" s="17">
+        <v>0</v>
+      </c>
+      <c r="T224" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="17">
+        <v>223</v>
+      </c>
+      <c r="B225" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C225" s="17">
+        <v>31.314731944444446</v>
+      </c>
+      <c r="D225" s="17">
+        <v>-92.443528333333333</v>
+      </c>
+      <c r="F225" s="17">
+        <v>0</v>
+      </c>
+      <c r="G225" s="17">
+        <v>0</v>
+      </c>
+      <c r="H225" s="17">
+        <v>0</v>
+      </c>
+      <c r="I225" s="17">
+        <v>0</v>
+      </c>
+      <c r="J225" s="17">
+        <v>0</v>
+      </c>
+      <c r="K225" s="17">
+        <v>0</v>
+      </c>
+      <c r="L225" s="17">
+        <v>0</v>
+      </c>
+      <c r="M225" s="17">
+        <v>0</v>
+      </c>
+      <c r="N225" s="17">
+        <v>0</v>
+      </c>
+      <c r="O225" s="17">
+        <v>0</v>
+      </c>
+      <c r="P225" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q225" s="17">
+        <v>0</v>
+      </c>
+      <c r="R225" s="17">
+        <v>0</v>
+      </c>
+      <c r="S225" s="17">
+        <v>0</v>
+      </c>
+      <c r="T225" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="17">
+        <v>224</v>
+      </c>
+      <c r="B226" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C226" s="17">
+        <v>31.111347222222225</v>
+      </c>
+      <c r="D226" s="17">
+        <v>-92.469453333333334</v>
+      </c>
+      <c r="F226" s="17">
+        <v>0</v>
+      </c>
+      <c r="G226" s="17">
+        <v>0</v>
+      </c>
+      <c r="H226" s="17">
+        <v>0</v>
+      </c>
+      <c r="I226" s="17">
+        <v>0</v>
+      </c>
+      <c r="J226" s="17">
+        <v>0</v>
+      </c>
+      <c r="K226" s="17">
+        <v>0</v>
+      </c>
+      <c r="L226" s="17">
+        <v>0</v>
+      </c>
+      <c r="M226" s="17">
+        <v>0</v>
+      </c>
+      <c r="N226" s="17">
+        <v>0</v>
+      </c>
+      <c r="O226" s="17">
+        <v>0</v>
+      </c>
+      <c r="P226" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q226" s="17">
+        <v>0</v>
+      </c>
+      <c r="R226" s="17">
+        <v>0</v>
+      </c>
+      <c r="S226" s="17">
+        <v>0</v>
+      </c>
+      <c r="T226" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="17">
+        <v>225</v>
+      </c>
+      <c r="B227" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C227" s="17">
+        <v>29.93311388888889</v>
+      </c>
+      <c r="D227" s="17">
+        <v>-93.079265277777779</v>
+      </c>
+    </row>
+    <row r="228" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="17">
+        <v>226</v>
+      </c>
+      <c r="B228" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C228" s="17">
+        <v>29.746413333333333</v>
+      </c>
+      <c r="D228" s="17">
+        <v>-92.324998888888885</v>
       </c>
     </row>
   </sheetData>
@@ -20770,30 +21765,30 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="17">
+      <c r="A34">
         <v>205</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34">
         <v>30.020377700000001</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34">
         <v>-90.142554000000004</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="17">
+      <c r="A35">
         <v>208</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35">
         <v>29.598918333333334</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35">
         <v>-90.710750000000004</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -21975,16 +22970,16 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="17">
+      <c r="A62">
         <v>176</v>
       </c>
-      <c r="B62" s="17">
+      <c r="B62">
         <v>30.258914999999998</v>
       </c>
-      <c r="C62" s="17">
+      <c r="C62">
         <v>-91.321944722222213</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -22003,16 +22998,16 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="17">
+      <c r="A64">
         <v>182</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64">
         <v>32.312416666666664</v>
       </c>
-      <c r="C64" s="17">
+      <c r="C64">
         <v>-92.443666666666672</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D64" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -22087,30 +23082,30 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="17">
+      <c r="A70">
         <v>209</v>
       </c>
-      <c r="B70" s="17">
+      <c r="B70">
         <v>29.578356111111113</v>
       </c>
-      <c r="C70" s="17">
+      <c r="C70">
         <v>-90.721383055555563</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D70" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="17">
+      <c r="A71">
         <v>211</v>
       </c>
-      <c r="B71" s="17">
+      <c r="B71">
         <v>29.561021111111113</v>
       </c>
-      <c r="C71" s="17">
+      <c r="C71">
         <v>-90.791579722222224</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D71" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated All Sites Google Map and added Online Donation Form coding to "Support the Hunt."
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/new_spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAFB4AC-E2FB-6C4E-94C8-31BBE5BB01A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735C2182-ECE6-4946-8425-8B129C8DE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="27">
   <si>
     <t>Long</t>
   </si>
@@ -191,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +201,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
@@ -264,6 +270,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L239"/>
+  <dimension ref="A1:L245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I239" sqref="I233:I239"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="E245" sqref="E245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4677,7 +4687,7 @@
         <v>15.49</v>
       </c>
       <c r="E136" s="3">
-        <f t="shared" ref="E136:E239" si="18">B136+C136/60+D136/3600</f>
+        <f t="shared" ref="E136:E245" si="18">B136+C136/60+D136/3600</f>
         <v>30.370969444444444</v>
       </c>
       <c r="F136" s="1">
@@ -4690,7 +4700,7 @@
         <v>31.54</v>
       </c>
       <c r="I136">
-        <f t="shared" ref="I136:I239" si="19">-F136-G136/60-H136/3600</f>
+        <f t="shared" ref="I136:I245" si="19">-F136-G136/60-H136/3600</f>
         <v>-91.625427777777773</v>
       </c>
     </row>
@@ -7885,6 +7895,192 @@
       <c r="I239">
         <f t="shared" si="19"/>
         <v>-92.028547500000002</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>234</v>
+      </c>
+      <c r="B240" s="1">
+        <v>29</v>
+      </c>
+      <c r="C240">
+        <v>52</v>
+      </c>
+      <c r="D240">
+        <v>57.81</v>
+      </c>
+      <c r="E240" s="3">
+        <f t="shared" si="18"/>
+        <v>29.882725000000001</v>
+      </c>
+      <c r="F240" s="1">
+        <v>90</v>
+      </c>
+      <c r="G240">
+        <v>25</v>
+      </c>
+      <c r="H240">
+        <v>55.774999999999999</v>
+      </c>
+      <c r="I240">
+        <f t="shared" si="19"/>
+        <v>-90.432159722222224</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>235</v>
+      </c>
+      <c r="B241" s="1">
+        <v>30</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+      <c r="D241">
+        <v>17.981999999999999</v>
+      </c>
+      <c r="E241" s="3">
+        <f t="shared" si="18"/>
+        <v>30.021661666666667</v>
+      </c>
+      <c r="F241" s="1">
+        <v>90</v>
+      </c>
+      <c r="G241">
+        <v>24</v>
+      </c>
+      <c r="H241">
+        <v>35.771000000000001</v>
+      </c>
+      <c r="I241">
+        <f t="shared" si="19"/>
+        <v>-90.409936388888894</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>236</v>
+      </c>
+      <c r="B242" s="1">
+        <v>30</v>
+      </c>
+      <c r="C242">
+        <v>2</v>
+      </c>
+      <c r="D242">
+        <v>10.744999999999999</v>
+      </c>
+      <c r="E242" s="3">
+        <f t="shared" si="18"/>
+        <v>30.036318055555558</v>
+      </c>
+      <c r="F242" s="1">
+        <v>90</v>
+      </c>
+      <c r="G242">
+        <v>25</v>
+      </c>
+      <c r="H242">
+        <v>55.944000000000003</v>
+      </c>
+      <c r="I242">
+        <f t="shared" si="19"/>
+        <v>-90.432206666666673</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>237</v>
+      </c>
+      <c r="B243" s="1">
+        <v>30</v>
+      </c>
+      <c r="C243">
+        <v>16</v>
+      </c>
+      <c r="D243">
+        <v>5.835</v>
+      </c>
+      <c r="E243" s="3">
+        <f t="shared" si="18"/>
+        <v>30.2682875</v>
+      </c>
+      <c r="F243" s="1">
+        <v>91</v>
+      </c>
+      <c r="G243">
+        <v>19</v>
+      </c>
+      <c r="H243">
+        <v>14.887</v>
+      </c>
+      <c r="I243">
+        <f t="shared" si="19"/>
+        <v>-91.32080194444444</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>238</v>
+      </c>
+      <c r="B244" s="1">
+        <v>30</v>
+      </c>
+      <c r="C244">
+        <v>9</v>
+      </c>
+      <c r="D244">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="E244" s="3">
+        <f t="shared" si="18"/>
+        <v>30.150213055555554</v>
+      </c>
+      <c r="F244" s="1">
+        <v>91</v>
+      </c>
+      <c r="G244">
+        <v>19</v>
+      </c>
+      <c r="H244">
+        <v>40.256</v>
+      </c>
+      <c r="I244">
+        <f t="shared" si="19"/>
+        <v>-91.32784888888888</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>239</v>
+      </c>
+      <c r="B245" s="1">
+        <v>30</v>
+      </c>
+      <c r="C245">
+        <v>8</v>
+      </c>
+      <c r="D245">
+        <v>53.387999999999998</v>
+      </c>
+      <c r="E245" s="3">
+        <f t="shared" si="18"/>
+        <v>30.148163333333333</v>
+      </c>
+      <c r="F245" s="1">
+        <v>91</v>
+      </c>
+      <c r="G245">
+        <v>19</v>
+      </c>
+      <c r="H245">
+        <v>45.902999999999999</v>
+      </c>
+      <c r="I245">
+        <f t="shared" si="19"/>
+        <v>-91.329417499999991</v>
       </c>
     </row>
   </sheetData>
@@ -9722,11 +9918,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U236"/>
+  <dimension ref="A1:U242"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E240" sqref="E240"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S241" sqref="S241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22027,6 +22223,270 @@
         <v>0</v>
       </c>
       <c r="T236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="17">
+        <v>234</v>
+      </c>
+      <c r="B237" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C237" s="17">
+        <v>29.882725000000001</v>
+      </c>
+      <c r="D237" s="17">
+        <v>-90.432159722222224</v>
+      </c>
+      <c r="F237" s="17">
+        <v>0</v>
+      </c>
+      <c r="G237" s="17">
+        <v>0</v>
+      </c>
+      <c r="H237" s="17">
+        <v>0</v>
+      </c>
+      <c r="I237" s="17">
+        <v>0</v>
+      </c>
+      <c r="J237" s="17">
+        <v>0</v>
+      </c>
+      <c r="K237" s="17">
+        <v>0</v>
+      </c>
+      <c r="L237" s="17">
+        <v>0</v>
+      </c>
+      <c r="M237" s="17">
+        <v>0</v>
+      </c>
+      <c r="N237" s="17">
+        <v>0</v>
+      </c>
+      <c r="O237" s="17">
+        <v>0</v>
+      </c>
+      <c r="P237" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q237" s="17">
+        <v>0</v>
+      </c>
+      <c r="R237" s="17">
+        <v>0</v>
+      </c>
+      <c r="S237" s="17">
+        <v>0</v>
+      </c>
+      <c r="T237" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="17">
+        <v>235</v>
+      </c>
+      <c r="B238" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C238" s="17">
+        <v>30.021661666666667</v>
+      </c>
+      <c r="D238" s="17">
+        <v>-90.409936388888894</v>
+      </c>
+    </row>
+    <row r="239" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="17">
+        <v>236</v>
+      </c>
+      <c r="B239" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C239" s="17">
+        <v>30.036318055555558</v>
+      </c>
+      <c r="D239" s="17">
+        <v>-90.432206666666673</v>
+      </c>
+    </row>
+    <row r="240" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="17">
+        <v>237</v>
+      </c>
+      <c r="B240" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C240" s="17">
+        <v>30.2682875</v>
+      </c>
+      <c r="D240" s="17">
+        <v>-91.32080194444444</v>
+      </c>
+      <c r="F240" s="17">
+        <v>0</v>
+      </c>
+      <c r="G240" s="17">
+        <v>0</v>
+      </c>
+      <c r="H240" s="17">
+        <v>0</v>
+      </c>
+      <c r="I240" s="17">
+        <v>0</v>
+      </c>
+      <c r="J240" s="17">
+        <v>0</v>
+      </c>
+      <c r="K240" s="17">
+        <v>0</v>
+      </c>
+      <c r="L240" s="17">
+        <v>0</v>
+      </c>
+      <c r="M240" s="17">
+        <v>0</v>
+      </c>
+      <c r="N240" s="17">
+        <v>0</v>
+      </c>
+      <c r="O240" s="17">
+        <v>0</v>
+      </c>
+      <c r="P240" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q240" s="17">
+        <v>0</v>
+      </c>
+      <c r="R240" s="17">
+        <v>0</v>
+      </c>
+      <c r="S240" s="17">
+        <v>0</v>
+      </c>
+      <c r="T240" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="17">
+        <v>238</v>
+      </c>
+      <c r="B241" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C241" s="17">
+        <v>30.150213055555554</v>
+      </c>
+      <c r="D241" s="17">
+        <v>-91.32784888888888</v>
+      </c>
+      <c r="F241" s="17">
+        <v>0</v>
+      </c>
+      <c r="G241" s="17">
+        <v>0</v>
+      </c>
+      <c r="H241" s="17">
+        <v>0</v>
+      </c>
+      <c r="I241" s="17">
+        <v>0</v>
+      </c>
+      <c r="J241" s="17">
+        <v>0</v>
+      </c>
+      <c r="K241" s="17">
+        <v>0</v>
+      </c>
+      <c r="L241" s="17">
+        <v>0</v>
+      </c>
+      <c r="M241" s="17">
+        <v>0</v>
+      </c>
+      <c r="N241" s="17">
+        <v>0</v>
+      </c>
+      <c r="O241" s="17">
+        <v>0</v>
+      </c>
+      <c r="P241" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q241" s="17">
+        <v>0</v>
+      </c>
+      <c r="R241" s="17">
+        <v>0</v>
+      </c>
+      <c r="S241" s="17">
+        <v>0</v>
+      </c>
+      <c r="T241" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="17">
+        <v>239</v>
+      </c>
+      <c r="B242" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C242" s="17">
+        <v>30.148163333333333</v>
+      </c>
+      <c r="D242" s="17">
+        <v>-91.329417499999991</v>
+      </c>
+      <c r="F242" s="17">
+        <v>0</v>
+      </c>
+      <c r="G242" s="17">
+        <v>0</v>
+      </c>
+      <c r="H242" s="17">
+        <v>0</v>
+      </c>
+      <c r="I242" s="17">
+        <v>0</v>
+      </c>
+      <c r="J242" s="17">
+        <v>0</v>
+      </c>
+      <c r="K242" s="17">
+        <v>0</v>
+      </c>
+      <c r="L242" s="17">
+        <v>0</v>
+      </c>
+      <c r="M242" s="17">
+        <v>0</v>
+      </c>
+      <c r="N242" s="17">
+        <v>0</v>
+      </c>
+      <c r="O242" s="17">
+        <v>0</v>
+      </c>
+      <c r="P242" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q242" s="17">
+        <v>0</v>
+      </c>
+      <c r="R242" s="17">
+        <v>0</v>
+      </c>
+      <c r="S242" s="17">
+        <v>0</v>
+      </c>
+      <c r="T242" s="17">
         <v>0</v>
       </c>
     </row>

</xml_diff>